<commit_message>
Updated timesheet from Martson Grind on 10/25
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_CarterKreis.xlsx
+++ b/Documentation/TimeSheets/TimeReport_CarterKreis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\plant-partner\Documentation\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731340B2-2179-4E22-A202-F66FD76CCDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56AAE82-15E2-42FF-8472-AB6A5E0F56C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2436" windowWidth="17280" windowHeight="8964" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Name:</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Repeated issues with recursively cloning the submodule esp-idf. Cloning into the submodule itself took 10-12 minutes and the first two times some of the directories failed to clone on time.</t>
+  </si>
+  <si>
+    <t>Finally got the ESP-IDF to flash ESP32 after switching to my Ubuntu OS. Proceeded to research and write the code to turn on external GPIO LED that is wired on breadboard and on-board LED. Also helped containerize, clean-up, and comment overall code for Pre-Alpha Build</t>
   </si>
 </sst>
 </file>
@@ -555,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,7 +585,7 @@
       </c>
       <c r="E1" s="4">
         <f>SUM(E4:E199)</f>
-        <v>0.39444444444444465</v>
+        <v>0.7118055555555558</v>
       </c>
       <c r="F1" s="5"/>
     </row>
@@ -740,14 +743,14 @@
         <v>17</v>
       </c>
       <c r="C10" s="15">
-        <v>0.10416666666666667</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D10" s="15">
-        <v>0.1701388888888889</v>
+        <v>0.67013888888888884</v>
       </c>
       <c r="E10" s="9">
         <f t="shared" ref="E10:E68" si="1">D10-C10</f>
-        <v>6.5972222222222224E-2</v>
+        <v>6.597222222222221E-2</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>19</v>
@@ -761,29 +764,39 @@
         <v>17</v>
       </c>
       <c r="C11" s="15">
-        <v>0.30208333333333331</v>
+        <v>0.80208333333333337</v>
       </c>
       <c r="D11" s="15">
-        <v>0.37361111111111112</v>
+        <v>0.87361111111111112</v>
       </c>
       <c r="E11" s="9">
         <f t="shared" si="1"/>
-        <v>7.1527777777777801E-2</v>
+        <v>7.1527777777777746E-2</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="A12" s="6">
+        <v>45955</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="15">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="D12" s="15">
+        <v>0.73750000000000004</v>
+      </c>
       <c r="E12" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="10"/>
+        <v>0.31736111111111115</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>

</xml_diff>

<commit_message>
Added PCB Design files into new pcbDesign Directory. Got ESP-IDF working on my Windows and figured out ESP-32 Model (I think 99% sure). Updated timesheets also
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_CarterKreis.xlsx
+++ b/Documentation/TimeSheets/TimeReport_CarterKreis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\plant-partner\Documentation\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56AAE82-15E2-42FF-8472-AB6A5E0F56C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D054D8E-66EB-4CD8-AD0C-93C13587A087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Name:</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>Finally got the ESP-IDF to flash ESP32 after switching to my Ubuntu OS. Proceeded to research and write the code to turn on external GPIO LED that is wired on breadboard and on-board LED. Also helped containerize, clean-up, and comment overall code for Pre-Alpha Build</t>
+  </si>
+  <si>
+    <t>Design Prototype</t>
+  </si>
+  <si>
+    <t>Worked on trying to get the specific ESP-32 model by analyzing the ESP32 info structs. I also got ESP-IDF working on Windows which needed some drivers uninstalled then proper ones re-installed</t>
+  </si>
+  <si>
+    <t>Setup KiCad for PCB Design. Throughout this week and the next, I will figure out specific footprints for out sensors and design the PCB Schematic and then PCB design</t>
   </si>
 </sst>
 </file>
@@ -178,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -210,9 +219,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -559,21 +565,21 @@
   <dimension ref="A1:F199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="166.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="244.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,11 +591,11 @@
       </c>
       <c r="E1" s="4">
         <f>SUM(E4:E199)</f>
-        <v>0.7118055555555558</v>
+        <v>0.82986111111111138</v>
       </c>
       <c r="F1" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -609,7 +615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>45933</v>
       </c>
@@ -630,7 +636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>45936</v>
       </c>
@@ -651,7 +657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>45942</v>
       </c>
@@ -672,7 +678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>45944</v>
       </c>
@@ -693,7 +699,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>45950</v>
       </c>
@@ -714,7 +720,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>45950</v>
       </c>
@@ -735,17 +741,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>45954</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="8">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="8">
         <v>0.67013888888888884</v>
       </c>
       <c r="E10" s="9">
@@ -756,17 +762,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>45954</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="8">
         <v>0.80208333333333337</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="8">
         <v>0.87361111111111112</v>
       </c>
       <c r="E11" s="9">
@@ -777,17 +783,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>45955</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="8">
         <v>0.4201388888888889</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="8">
         <v>0.73750000000000004</v>
       </c>
       <c r="E12" s="9">
@@ -798,29 +804,49 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>45965</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.37847222222222221</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.46180555555555558</v>
+      </c>
       <c r="E13" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>45965</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.60763888888888884</v>
+      </c>
       <c r="E14" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -831,7 +857,7 @@
       </c>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -842,7 +868,7 @@
       </c>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -853,7 +879,7 @@
       </c>
       <c r="F17" s="10"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -864,7 +890,7 @@
       </c>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -875,7 +901,7 @@
       </c>
       <c r="F19" s="10"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -886,7 +912,7 @@
       </c>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -897,7 +923,7 @@
       </c>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -908,7 +934,7 @@
       </c>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -919,7 +945,7 @@
       </c>
       <c r="F23" s="10"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -930,7 +956,7 @@
       </c>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -941,7 +967,7 @@
       </c>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -952,7 +978,7 @@
       </c>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -963,7 +989,7 @@
       </c>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -974,7 +1000,7 @@
       </c>
       <c r="F28" s="10"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -985,7 +1011,7 @@
       </c>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -996,7 +1022,7 @@
       </c>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1007,7 +1033,7 @@
       </c>
       <c r="F31" s="10"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1018,7 +1044,7 @@
       </c>
       <c r="F32" s="10"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1029,7 +1055,7 @@
       </c>
       <c r="F33" s="10"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1040,7 +1066,7 @@
       </c>
       <c r="F34" s="10"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1051,7 +1077,7 @@
       </c>
       <c r="F35" s="10"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1062,7 +1088,7 @@
       </c>
       <c r="F36" s="10"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1073,7 +1099,7 @@
       </c>
       <c r="F37" s="10"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1084,7 +1110,7 @@
       </c>
       <c r="F38" s="10"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1095,7 +1121,7 @@
       </c>
       <c r="F39" s="10"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1106,7 +1132,7 @@
       </c>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1117,7 +1143,7 @@
       </c>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1128,7 +1154,7 @@
       </c>
       <c r="F42" s="10"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1139,7 +1165,7 @@
       </c>
       <c r="F43" s="10"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1150,7 +1176,7 @@
       </c>
       <c r="F44" s="10"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1161,7 +1187,7 @@
       </c>
       <c r="F45" s="10"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1172,7 +1198,7 @@
       </c>
       <c r="F46" s="10"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1183,7 +1209,7 @@
       </c>
       <c r="F47" s="10"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1194,7 +1220,7 @@
       </c>
       <c r="F48" s="10"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1205,7 +1231,7 @@
       </c>
       <c r="F49" s="10"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1216,7 +1242,7 @@
       </c>
       <c r="F50" s="10"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1227,7 +1253,7 @@
       </c>
       <c r="F51" s="10"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1238,7 +1264,7 @@
       </c>
       <c r="F52" s="10"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1249,7 +1275,7 @@
       </c>
       <c r="F53" s="10"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -1260,7 +1286,7 @@
       </c>
       <c r="F54" s="10"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1271,7 +1297,7 @@
       </c>
       <c r="F55" s="10"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1282,7 +1308,7 @@
       </c>
       <c r="F56" s="10"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -1293,7 +1319,7 @@
       </c>
       <c r="F57" s="10"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -1304,7 +1330,7 @@
       </c>
       <c r="F58" s="10"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -1315,7 +1341,7 @@
       </c>
       <c r="F59" s="10"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1326,7 +1352,7 @@
       </c>
       <c r="F60" s="10"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1337,7 +1363,7 @@
       </c>
       <c r="F61" s="10"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1348,7 +1374,7 @@
       </c>
       <c r="F62" s="10"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1359,7 +1385,7 @@
       </c>
       <c r="F63" s="10"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1370,7 +1396,7 @@
       </c>
       <c r="F64" s="10"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1381,7 +1407,7 @@
       </c>
       <c r="F65" s="10"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1392,7 +1418,7 @@
       </c>
       <c r="F66" s="10"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1403,7 +1429,7 @@
       </c>
       <c r="F67" s="10"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1414,7 +1440,7 @@
       </c>
       <c r="F68" s="10"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -1425,7 +1451,7 @@
       </c>
       <c r="F69" s="10"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -1436,7 +1462,7 @@
       </c>
       <c r="F70" s="10"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1447,7 +1473,7 @@
       </c>
       <c r="F71" s="10"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1458,7 +1484,7 @@
       </c>
       <c r="F72" s="10"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -1469,7 +1495,7 @@
       </c>
       <c r="F73" s="10"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -1480,7 +1506,7 @@
       </c>
       <c r="F74" s="10"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -1491,7 +1517,7 @@
       </c>
       <c r="F75" s="10"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -1502,7 +1528,7 @@
       </c>
       <c r="F76" s="10"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -1513,7 +1539,7 @@
       </c>
       <c r="F77" s="10"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -1524,7 +1550,7 @@
       </c>
       <c r="F78" s="10"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -1535,7 +1561,7 @@
       </c>
       <c r="F79" s="10"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -1546,7 +1572,7 @@
       </c>
       <c r="F80" s="10"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -1557,7 +1583,7 @@
       </c>
       <c r="F81" s="10"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1568,7 +1594,7 @@
       </c>
       <c r="F82" s="10"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -1579,7 +1605,7 @@
       </c>
       <c r="F83" s="10"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -1590,7 +1616,7 @@
       </c>
       <c r="F84" s="10"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -1601,7 +1627,7 @@
       </c>
       <c r="F85" s="10"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -1612,7 +1638,7 @@
       </c>
       <c r="F86" s="10"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -1623,7 +1649,7 @@
       </c>
       <c r="F87" s="10"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -1634,7 +1660,7 @@
       </c>
       <c r="F88" s="10"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -1645,7 +1671,7 @@
       </c>
       <c r="F89" s="10"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1656,7 +1682,7 @@
       </c>
       <c r="F90" s="10"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -1667,7 +1693,7 @@
       </c>
       <c r="F91" s="10"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -1678,7 +1704,7 @@
       </c>
       <c r="F92" s="10"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -1689,7 +1715,7 @@
       </c>
       <c r="F93" s="10"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -1700,7 +1726,7 @@
       </c>
       <c r="F94" s="10"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -1711,7 +1737,7 @@
       </c>
       <c r="F95" s="10"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -1722,7 +1748,7 @@
       </c>
       <c r="F96" s="10"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -1733,7 +1759,7 @@
       </c>
       <c r="F97" s="10"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -1744,7 +1770,7 @@
       </c>
       <c r="F98" s="10"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -1755,7 +1781,7 @@
       </c>
       <c r="F99" s="10"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -1766,7 +1792,7 @@
       </c>
       <c r="F100" s="10"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -1777,7 +1803,7 @@
       </c>
       <c r="F101" s="10"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -1788,7 +1814,7 @@
       </c>
       <c r="F102" s="10"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -1799,7 +1825,7 @@
       </c>
       <c r="F103" s="10"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -1810,7 +1836,7 @@
       </c>
       <c r="F104" s="10"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -1821,7 +1847,7 @@
       </c>
       <c r="F105" s="10"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -1832,7 +1858,7 @@
       </c>
       <c r="F106" s="10"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -1843,7 +1869,7 @@
       </c>
       <c r="F107" s="10"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -1854,7 +1880,7 @@
       </c>
       <c r="F108" s="10"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -1865,7 +1891,7 @@
       </c>
       <c r="F109" s="10"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -1876,7 +1902,7 @@
       </c>
       <c r="F110" s="10"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -1887,7 +1913,7 @@
       </c>
       <c r="F111" s="10"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -1898,7 +1924,7 @@
       </c>
       <c r="F112" s="10"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -1909,7 +1935,7 @@
       </c>
       <c r="F113" s="10"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -1920,7 +1946,7 @@
       </c>
       <c r="F114" s="10"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -1931,7 +1957,7 @@
       </c>
       <c r="F115" s="10"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -1942,7 +1968,7 @@
       </c>
       <c r="F116" s="10"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -1953,7 +1979,7 @@
       </c>
       <c r="F117" s="10"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -1964,7 +1990,7 @@
       </c>
       <c r="F118" s="10"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -1975,7 +2001,7 @@
       </c>
       <c r="F119" s="10"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -1986,7 +2012,7 @@
       </c>
       <c r="F120" s="10"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -1997,7 +2023,7 @@
       </c>
       <c r="F121" s="10"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -2008,7 +2034,7 @@
       </c>
       <c r="F122" s="10"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -2019,7 +2045,7 @@
       </c>
       <c r="F123" s="10"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -2030,7 +2056,7 @@
       </c>
       <c r="F124" s="10"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>
@@ -2041,7 +2067,7 @@
       </c>
       <c r="F125" s="10"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
@@ -2052,7 +2078,7 @@
       </c>
       <c r="F126" s="10"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="7"/>
       <c r="B127" s="7"/>
       <c r="C127" s="7"/>
@@ -2063,7 +2089,7 @@
       </c>
       <c r="F127" s="10"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="7"/>
       <c r="B128" s="7"/>
       <c r="C128" s="7"/>
@@ -2074,7 +2100,7 @@
       </c>
       <c r="F128" s="10"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="7"/>
@@ -2085,7 +2111,7 @@
       </c>
       <c r="F129" s="10"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
@@ -2096,7 +2122,7 @@
       </c>
       <c r="F130" s="10"/>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="7"/>
@@ -2107,7 +2133,7 @@
       </c>
       <c r="F131" s="10"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
@@ -2118,7 +2144,7 @@
       </c>
       <c r="F132" s="10"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="7"/>
@@ -2129,7 +2155,7 @@
       </c>
       <c r="F133" s="10"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
@@ -2140,7 +2166,7 @@
       </c>
       <c r="F134" s="10"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
@@ -2151,7 +2177,7 @@
       </c>
       <c r="F135" s="10"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
@@ -2162,7 +2188,7 @@
       </c>
       <c r="F136" s="10"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
       <c r="C137" s="7"/>
@@ -2173,7 +2199,7 @@
       </c>
       <c r="F137" s="10"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
@@ -2184,7 +2210,7 @@
       </c>
       <c r="F138" s="10"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
@@ -2195,7 +2221,7 @@
       </c>
       <c r="F139" s="10"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
@@ -2206,7 +2232,7 @@
       </c>
       <c r="F140" s="10"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
@@ -2217,7 +2243,7 @@
       </c>
       <c r="F141" s="10"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="7"/>
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
@@ -2228,7 +2254,7 @@
       </c>
       <c r="F142" s="10"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="7"/>
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
@@ -2239,7 +2265,7 @@
       </c>
       <c r="F143" s="10"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="7"/>
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
@@ -2250,7 +2276,7 @@
       </c>
       <c r="F144" s="10"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
@@ -2261,7 +2287,7 @@
       </c>
       <c r="F145" s="10"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="7"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
@@ -2272,7 +2298,7 @@
       </c>
       <c r="F146" s="10"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="7"/>
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
@@ -2283,7 +2309,7 @@
       </c>
       <c r="F147" s="10"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="7"/>
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
@@ -2294,7 +2320,7 @@
       </c>
       <c r="F148" s="10"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="7"/>
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
@@ -2305,7 +2331,7 @@
       </c>
       <c r="F149" s="10"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="7"/>
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
@@ -2316,7 +2342,7 @@
       </c>
       <c r="F150" s="10"/>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="7"/>
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
@@ -2327,7 +2353,7 @@
       </c>
       <c r="F151" s="10"/>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="7"/>
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
@@ -2338,7 +2364,7 @@
       </c>
       <c r="F152" s="10"/>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="7"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
@@ -2349,7 +2375,7 @@
       </c>
       <c r="F153" s="10"/>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="7"/>
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
@@ -2360,7 +2386,7 @@
       </c>
       <c r="F154" s="10"/>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="7"/>
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
@@ -2371,7 +2397,7 @@
       </c>
       <c r="F155" s="10"/>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="7"/>
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
@@ -2382,7 +2408,7 @@
       </c>
       <c r="F156" s="10"/>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="7"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
@@ -2393,7 +2419,7 @@
       </c>
       <c r="F157" s="10"/>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="7"/>
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
@@ -2404,7 +2430,7 @@
       </c>
       <c r="F158" s="10"/>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="7"/>
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
@@ -2415,7 +2441,7 @@
       </c>
       <c r="F159" s="10"/>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="7"/>
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
@@ -2426,7 +2452,7 @@
       </c>
       <c r="F160" s="10"/>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="7"/>
       <c r="B161" s="7"/>
       <c r="C161" s="7"/>
@@ -2437,7 +2463,7 @@
       </c>
       <c r="F161" s="10"/>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
@@ -2448,7 +2474,7 @@
       </c>
       <c r="F162" s="10"/>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="7"/>
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
@@ -2459,7 +2485,7 @@
       </c>
       <c r="F163" s="10"/>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
@@ -2470,7 +2496,7 @@
       </c>
       <c r="F164" s="10"/>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="7"/>
       <c r="B165" s="7"/>
       <c r="C165" s="7"/>
@@ -2481,7 +2507,7 @@
       </c>
       <c r="F165" s="10"/>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
@@ -2492,7 +2518,7 @@
       </c>
       <c r="F166" s="10"/>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="7"/>
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
@@ -2503,7 +2529,7 @@
       </c>
       <c r="F167" s="10"/>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
@@ -2514,7 +2540,7 @@
       </c>
       <c r="F168" s="10"/>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="7"/>
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
@@ -2525,7 +2551,7 @@
       </c>
       <c r="F169" s="10"/>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
@@ -2536,7 +2562,7 @@
       </c>
       <c r="F170" s="10"/>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="7"/>
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
@@ -2547,7 +2573,7 @@
       </c>
       <c r="F171" s="10"/>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
@@ -2558,7 +2584,7 @@
       </c>
       <c r="F172" s="10"/>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="7"/>
       <c r="B173" s="7"/>
       <c r="C173" s="7"/>
@@ -2569,7 +2595,7 @@
       </c>
       <c r="F173" s="10"/>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="7"/>
       <c r="B174" s="7"/>
       <c r="C174" s="7"/>
@@ -2580,7 +2606,7 @@
       </c>
       <c r="F174" s="10"/>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="7"/>
       <c r="B175" s="7"/>
       <c r="C175" s="7"/>
@@ -2591,7 +2617,7 @@
       </c>
       <c r="F175" s="10"/>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="7"/>
       <c r="B176" s="7"/>
       <c r="C176" s="7"/>
@@ -2602,7 +2628,7 @@
       </c>
       <c r="F176" s="10"/>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="7"/>
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
@@ -2613,7 +2639,7 @@
       </c>
       <c r="F177" s="10"/>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="7"/>
       <c r="B178" s="7"/>
       <c r="C178" s="7"/>
@@ -2624,7 +2650,7 @@
       </c>
       <c r="F178" s="10"/>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="7"/>
       <c r="B179" s="7"/>
       <c r="C179" s="7"/>
@@ -2635,7 +2661,7 @@
       </c>
       <c r="F179" s="10"/>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="7"/>
       <c r="B180" s="7"/>
       <c r="C180" s="7"/>
@@ -2646,7 +2672,7 @@
       </c>
       <c r="F180" s="10"/>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="7"/>
       <c r="B181" s="7"/>
       <c r="C181" s="7"/>
@@ -2657,7 +2683,7 @@
       </c>
       <c r="F181" s="10"/>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="7"/>
       <c r="B182" s="7"/>
       <c r="C182" s="7"/>
@@ -2668,7 +2694,7 @@
       </c>
       <c r="F182" s="10"/>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="7"/>
       <c r="B183" s="7"/>
       <c r="C183" s="7"/>
@@ -2679,7 +2705,7 @@
       </c>
       <c r="F183" s="10"/>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="7"/>
       <c r="B184" s="7"/>
       <c r="C184" s="7"/>
@@ -2690,7 +2716,7 @@
       </c>
       <c r="F184" s="10"/>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="7"/>
       <c r="B185" s="7"/>
       <c r="C185" s="7"/>
@@ -2701,7 +2727,7 @@
       </c>
       <c r="F185" s="10"/>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="7"/>
       <c r="B186" s="7"/>
       <c r="C186" s="7"/>
@@ -2712,7 +2738,7 @@
       </c>
       <c r="F186" s="10"/>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="7"/>
       <c r="B187" s="7"/>
       <c r="C187" s="7"/>
@@ -2723,7 +2749,7 @@
       </c>
       <c r="F187" s="10"/>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="7"/>
       <c r="B188" s="7"/>
       <c r="C188" s="7"/>
@@ -2734,7 +2760,7 @@
       </c>
       <c r="F188" s="10"/>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="7"/>
       <c r="B189" s="7"/>
       <c r="C189" s="7"/>
@@ -2745,7 +2771,7 @@
       </c>
       <c r="F189" s="10"/>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="7"/>
       <c r="B190" s="7"/>
       <c r="C190" s="7"/>
@@ -2756,7 +2782,7 @@
       </c>
       <c r="F190" s="10"/>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="7"/>
       <c r="B191" s="7"/>
       <c r="C191" s="7"/>
@@ -2767,7 +2793,7 @@
       </c>
       <c r="F191" s="10"/>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="7"/>
       <c r="B192" s="7"/>
       <c r="C192" s="7"/>
@@ -2778,7 +2804,7 @@
       </c>
       <c r="F192" s="10"/>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="7"/>
       <c r="B193" s="7"/>
       <c r="C193" s="7"/>
@@ -2789,7 +2815,7 @@
       </c>
       <c r="F193" s="10"/>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="7"/>
       <c r="B194" s="7"/>
       <c r="C194" s="7"/>
@@ -2800,7 +2826,7 @@
       </c>
       <c r="F194" s="10"/>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="7"/>
       <c r="B195" s="7"/>
       <c r="C195" s="7"/>
@@ -2811,7 +2837,7 @@
       </c>
       <c r="F195" s="10"/>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="7"/>
       <c r="B196" s="7"/>
       <c r="C196" s="7"/>
@@ -2822,7 +2848,7 @@
       </c>
       <c r="F196" s="10"/>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="7"/>
       <c r="B197" s="7"/>
       <c r="C197" s="7"/>
@@ -2833,7 +2859,7 @@
       </c>
       <c r="F197" s="10"/>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="7"/>
       <c r="B198" s="7"/>
       <c r="C198" s="7"/>
@@ -2844,7 +2870,7 @@
       </c>
       <c r="F198" s="10"/>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="7"/>
       <c r="B199" s="7"/>
       <c r="C199" s="7"/>

</xml_diff>

<commit_message>
Carter updated his timesheet
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_CarterKreis.xlsx
+++ b/Documentation/TimeSheets/TimeReport_CarterKreis.xlsx
@@ -1,137 +1,148 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\plant-partner\Documentation\TimeSheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D054D8E-66EB-4CD8-AD0C-93C13587A087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
-    <t>Name:</t>
+    <t xml:space="preserve">Name:</t>
   </si>
   <si>
-    <t>Date:</t>
+    <t xml:space="preserve">Carter Kreis</t>
   </si>
   <si>
-    <t>Starting Time:</t>
+    <t xml:space="preserve">Total Time:</t>
   </si>
   <si>
-    <t>Ending  Time:</t>
+    <t xml:space="preserve">Date:</t>
   </si>
   <si>
-    <t>Calculated Time Worked:</t>
+    <t xml:space="preserve">General Category:</t>
   </si>
   <si>
-    <t>Description:</t>
+    <t xml:space="preserve">Starting Time:</t>
   </si>
   <si>
-    <t>Check-in</t>
+    <t xml:space="preserve">Ending  Time:</t>
   </si>
   <si>
-    <t>Design Draft</t>
+    <t xml:space="preserve">Calculated Time Worked:</t>
   </si>
   <si>
-    <t>General Category:</t>
+    <t xml:space="preserve">Description:</t>
   </si>
   <si>
-    <t>Sat down with group after class to define project and  talk through all of Design Draft points (Deliverables, Requirements, Division of work, ect.)</t>
+    <t xml:space="preserve">Design Draft</t>
   </si>
   <si>
-    <t>Total Time:</t>
+    <t xml:space="preserve">Sat down with group after class to define project and  talk through all of Design Draft points (Deliverables, Requirements, Division of work, ect.)</t>
   </si>
   <si>
-    <t>Carter Kreis</t>
+    <t xml:space="preserve">Check-in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check-in 1: Met with group &amp; Tyler. Discussed our design draft, and asked questions regarding design plan and material buying</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Researched and implemented Github webhook which sends all updates from Github to Discord channel named github-updates</t>
   </si>
   <si>
     <t xml:space="preserve">Check-in 2: Met with group &amp; Tyler. Reviewed out submitted design draft, discussed adding more hardware specification, and discussed with  group members to start buying materials and beginning research </t>
   </si>
   <si>
-    <t>Check-in 1: Met with group &amp; Tyler. Discussed our design draft, and asked questions regarding design plan and material buying</t>
+    <t xml:space="preserve">Check-in 3: Met with group &amp; Tyler. Planned out pre-alpha build documentation, materials list, and basic codebase structure. I will be working on PCB Design and physical materials for prototypes</t>
   </si>
   <si>
-    <t>Project Organization</t>
+    <t xml:space="preserve">Pre-Alpha Build</t>
   </si>
   <si>
-    <t>Researched and implemented Github webhook which sends all updates from Github to Discord channel named github-updates</t>
+    <t xml:space="preserve">Researched and begun setup of ESP-IDF through its VS Code extension</t>
   </si>
   <si>
-    <t>Check-in 3: Met with group &amp; Tyler. Planned out pre-alpha build documentation, materials list, and basic codebase structure. I will be working on PCB Design and physical materials for prototypes</t>
+    <t xml:space="preserve">Setup ESP-IDF extension in VS Code. Attempted Hello World example code but my laptop is not detecting ESP32 as a COM Port. We also continued to plan Pre-Alpha Build goal</t>
   </si>
   <si>
-    <t>Pre-Alpha Build</t>
+    <t xml:space="preserve">Repeated issues with recursively cloning the submodule esp-idf. Cloning into the submodule itself took 10-12 minutes and the first two times some of the directories failed to clone on time.</t>
   </si>
   <si>
-    <t>Researched and begun setup of ESP-IDF through its VS Code extension</t>
+    <t xml:space="preserve">Finally got the ESP-IDF to flash ESP32 after switching to my Ubuntu OS. Proceeded to research and write the code to turn on external GPIO LED that is wired on breadboard and on-board LED. Also helped containerize, clean-up, and comment overall code for Pre-Alpha Build</t>
   </si>
   <si>
-    <t>Setup ESP-IDF extension in VS Code. Attempted Hello World example code but my laptop is not detecting ESP32 as a COM Port. We also continued to plan Pre-Alpha Build goal</t>
+    <t xml:space="preserve">Design Prototype</t>
   </si>
   <si>
-    <t>Repeated issues with recursively cloning the submodule esp-idf. Cloning into the submodule itself took 10-12 minutes and the first two times some of the directories failed to clone on time.</t>
+    <t xml:space="preserve">Worked on trying to get the specific ESP-32 model by analyzing the ESP32 info structs. I also got ESP-IDF working on Windows which needed some drivers uninstalled then proper ones re-installed</t>
   </si>
   <si>
-    <t>Finally got the ESP-IDF to flash ESP32 after switching to my Ubuntu OS. Proceeded to research and write the code to turn on external GPIO LED that is wired on breadboard and on-board LED. Also helped containerize, clean-up, and comment overall code for Pre-Alpha Build</t>
+    <t xml:space="preserve">Setup KiCad for PCB Design. Throughout this week and the next, I will figure out specific footprints for out sensors and design the PCB Schematic and then PCB design</t>
   </si>
   <si>
-    <t>Design Prototype</t>
-  </si>
-  <si>
-    <t>Worked on trying to get the specific ESP-32 model by analyzing the ESP32 info structs. I also got ESP-IDF working on Windows which needed some drivers uninstalled then proper ones re-installed</t>
-  </si>
-  <si>
-    <t>Setup KiCad for PCB Design. Throughout this week and the next, I will figure out specific footprints for out sensors and design the PCB Schematic and then PCB design</t>
+    <t xml:space="preserve">Searched for and found my Infinity Stones (the schematics for each sensor for our PCB). Now that I gathered the schematics, I can start designing the PCB layout and how it will fit into our overall project and Design Prototype</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="7">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="[h]:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="167" formatCode="h:mm\ AM/PM"/>
+    <numFmt numFmtId="168" formatCode="h:mm:ss"/>
+    <numFmt numFmtId="169" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="170" formatCode="hh:mm\ AM/PM"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -143,298 +154,297 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="4" tint="0.7999"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF7FCFF"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFF7FCFF"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="2">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="46" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="46" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+  <cellXfs count="17">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="21" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <mruColors>
-      <color rgb="FFF7FCFF"/>
-      <color rgb="FFE5F5FF"/>
-      <color rgb="FFCCECFF"/>
-    </mruColors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFF7FCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFC1E5F5"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="0e2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="e8e8e8"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="e97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="196b24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="0f9ed5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="a02b93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="4ea72e"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="96607d"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
@@ -442,33 +452,24 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
@@ -481,13 +482,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -497,15 +492,13 @@
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:tint val="95000"/>
-            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
-                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
@@ -513,7 +506,6 @@
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
-                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
@@ -521,2368 +513,2359 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="63000"/>
-                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="244.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="244.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="1" width="8.86"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="n">
+        <f aca="false">SUM(E4:E199)</f>
+        <v>0.990972222222222</v>
+      </c>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="n">
+        <v>45933</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>0.470138888888889</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>0.610416666666667</v>
+      </c>
+      <c r="E4" s="9" t="n">
+        <f aca="false">D4-C4</f>
+        <v>0.140277777777778</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="n">
+        <v>45936</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="4">
-        <f>SUM(E4:E199)</f>
-        <v>0.82986111111111138</v>
-      </c>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>45933</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="8">
-        <v>0.47013888888888888</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0.61041666666666672</v>
-      </c>
-      <c r="E4" s="9">
-        <f t="shared" ref="E4:E9" si="0">D4-C4</f>
-        <v>0.14027777777777783</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>45936</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="C5" s="8" t="n">
         <v>0.625</v>
       </c>
-      <c r="D5" s="8">
-        <v>0.64722222222222225</v>
-      </c>
-      <c r="E5" s="9">
-        <f t="shared" si="0"/>
-        <v>2.2222222222222254E-2</v>
+      <c r="D5" s="8" t="n">
+        <v>0.647222222222222</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <f aca="false">D5-C5</f>
+        <v>0.0222222222222222</v>
       </c>
       <c r="F5" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="n">
+        <v>45942</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
-        <v>45942</v>
-      </c>
-      <c r="B6" s="12" t="s">
+      <c r="C6" s="13" t="n">
+        <v>0.803472222222222</v>
+      </c>
+      <c r="D6" s="13" t="n">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="E6" s="14" t="n">
+        <f aca="false">D6-C6</f>
+        <v>0.0298611111111111</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="13">
-        <v>0.80347222222222225</v>
-      </c>
-      <c r="D6" s="13">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E6" s="14">
-        <f t="shared" si="0"/>
-        <v>2.9861111111111116E-2</v>
-      </c>
-      <c r="F6" s="3" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="n">
+        <v>45944</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>0.472222222222222</v>
+      </c>
+      <c r="D7" s="8" t="n">
+        <v>0.49375</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <f aca="false">D7-C7</f>
+        <v>0.0215277777777778</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>45944</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0.47222222222222221</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.49375000000000002</v>
-      </c>
-      <c r="E7" s="9">
-        <f t="shared" si="0"/>
-        <v>2.1527777777777812E-2</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="n">
         <v>45950</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="8">
+        <v>11</v>
+      </c>
+      <c r="C8" s="8" t="n">
         <v>0.625</v>
       </c>
-      <c r="D8" s="8">
-        <v>0.64722222222222225</v>
-      </c>
-      <c r="E8" s="9">
-        <f t="shared" si="0"/>
-        <v>2.2222222222222254E-2</v>
+      <c r="D8" s="8" t="n">
+        <v>0.647222222222222</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <f aca="false">D8-C8</f>
+        <v>0.0222222222222222</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="n">
         <v>45950</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="8" t="n">
         <v>0.90625</v>
       </c>
-      <c r="D9" s="8">
-        <v>0.92708333333333337</v>
-      </c>
-      <c r="E9" s="9">
-        <f t="shared" si="0"/>
-        <v>2.083333333333337E-2</v>
+      <c r="D9" s="8" t="n">
+        <v>0.927083333333333</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <f aca="false">D9-C9</f>
+        <v>0.0208333333333333</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="n">
         <v>45954</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="8">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0.67013888888888884</v>
-      </c>
-      <c r="E10" s="9">
-        <f t="shared" ref="E10:E68" si="1">D10-C10</f>
-        <v>6.597222222222221E-2</v>
+      <c r="C10" s="8" t="n">
+        <v>0.604166666666667</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>0.670138888888889</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <f aca="false">D10-C10</f>
+        <v>0.0659722222222222</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="n">
         <v>45954</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="8">
-        <v>0.80208333333333337</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0.87361111111111112</v>
-      </c>
-      <c r="E11" s="9">
-        <f t="shared" si="1"/>
-        <v>7.1527777777777746E-2</v>
+      <c r="C11" s="8" t="n">
+        <v>0.802083333333333</v>
+      </c>
+      <c r="D11" s="8" t="n">
+        <v>0.873611111111111</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <f aca="false">D11-C11</f>
+        <v>0.0715277777777778</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="n">
         <v>45955</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="8">
-        <v>0.4201388888888889</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0.73750000000000004</v>
-      </c>
-      <c r="E12" s="9">
-        <f t="shared" si="1"/>
-        <v>0.31736111111111115</v>
+      <c r="C12" s="8" t="n">
+        <v>0.420138888888889</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <v>0.7375</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <f aca="false">D12-C12</f>
+        <v>0.317361111111111</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="n">
         <v>45965</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="8">
-        <v>0.37847222222222221</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0.46180555555555558</v>
-      </c>
-      <c r="E13" s="9">
-        <f t="shared" si="1"/>
-        <v>8.333333333333337E-2</v>
+      <c r="C13" s="8" t="n">
+        <v>0.378472222222222</v>
+      </c>
+      <c r="D13" s="8" t="n">
+        <v>0.461805555555556</v>
+      </c>
+      <c r="E13" s="9" t="n">
+        <f aca="false">D13-C13</f>
+        <v>0.0833333333333333</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="n">
         <v>45965</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="8">
-        <v>0.57291666666666663</v>
-      </c>
-      <c r="D14" s="8">
-        <v>0.60763888888888884</v>
-      </c>
-      <c r="E14" s="9">
-        <f t="shared" si="1"/>
-        <v>3.472222222222221E-2</v>
+      <c r="C14" s="8" t="n">
+        <v>0.572916666666667</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <v>0.607638888888889</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <f aca="false">D14-C14</f>
+        <v>0.0347222222222222</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="n">
+        <v>45967</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="16" t="n">
+        <v>0.420138888888889</v>
+      </c>
+      <c r="D15" s="16" t="n">
+        <v>0.58125</v>
+      </c>
+      <c r="E15" s="9" t="n">
+        <f aca="false">D15-C15</f>
+        <v>0.161111111111111</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="9">
-        <f t="shared" si="1"/>
+      <c r="E16" s="9" t="n">
+        <f aca="false">D16-C16</f>
         <v>0</v>
       </c>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="9">
-        <f t="shared" si="1"/>
+      <c r="E17" s="9" t="n">
+        <f aca="false">D17-C17</f>
         <v>0</v>
       </c>
       <c r="F17" s="10"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="9">
-        <f t="shared" si="1"/>
+      <c r="E18" s="9" t="n">
+        <f aca="false">D18-C18</f>
         <v>0</v>
       </c>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="9">
-        <f t="shared" si="1"/>
+      <c r="E19" s="9" t="n">
+        <f aca="false">D19-C19</f>
         <v>0</v>
       </c>
       <c r="F19" s="10"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="9">
-        <f t="shared" si="1"/>
+      <c r="E20" s="9" t="n">
+        <f aca="false">D20-C20</f>
         <v>0</v>
       </c>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="9">
-        <f t="shared" si="1"/>
+      <c r="E21" s="9" t="n">
+        <f aca="false">D21-C21</f>
         <v>0</v>
       </c>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="9">
-        <f t="shared" si="1"/>
+      <c r="E22" s="9" t="n">
+        <f aca="false">D22-C22</f>
         <v>0</v>
       </c>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="9">
-        <f t="shared" si="1"/>
+      <c r="E23" s="9" t="n">
+        <f aca="false">D23-C23</f>
         <v>0</v>
       </c>
       <c r="F23" s="10"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="9">
-        <f t="shared" si="1"/>
+      <c r="E24" s="9" t="n">
+        <f aca="false">D24-C24</f>
         <v>0</v>
       </c>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="9">
-        <f t="shared" si="1"/>
+      <c r="E25" s="9" t="n">
+        <f aca="false">D25-C25</f>
         <v>0</v>
       </c>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
-      <c r="E26" s="9">
-        <f t="shared" si="1"/>
+      <c r="E26" s="9" t="n">
+        <f aca="false">D26-C26</f>
         <v>0</v>
       </c>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="9">
-        <f t="shared" si="1"/>
+      <c r="E27" s="9" t="n">
+        <f aca="false">D27-C27</f>
         <v>0</v>
       </c>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
-      <c r="E28" s="9">
-        <f t="shared" si="1"/>
+      <c r="E28" s="9" t="n">
+        <f aca="false">D28-C28</f>
         <v>0</v>
       </c>
       <c r="F28" s="10"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="9">
-        <f t="shared" si="1"/>
+      <c r="E29" s="9" t="n">
+        <f aca="false">D29-C29</f>
         <v>0</v>
       </c>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
-      <c r="E30" s="9">
-        <f t="shared" si="1"/>
+      <c r="E30" s="9" t="n">
+        <f aca="false">D30-C30</f>
         <v>0</v>
       </c>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
-      <c r="E31" s="9">
-        <f t="shared" si="1"/>
+      <c r="E31" s="9" t="n">
+        <f aca="false">D31-C31</f>
         <v>0</v>
       </c>
       <c r="F31" s="10"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
-      <c r="E32" s="9">
-        <f t="shared" si="1"/>
+      <c r="E32" s="9" t="n">
+        <f aca="false">D32-C32</f>
         <v>0</v>
       </c>
       <c r="F32" s="10"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
-      <c r="E33" s="9">
-        <f t="shared" si="1"/>
+      <c r="E33" s="9" t="n">
+        <f aca="false">D33-C33</f>
         <v>0</v>
       </c>
       <c r="F33" s="10"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
-      <c r="E34" s="9">
-        <f t="shared" si="1"/>
+      <c r="E34" s="9" t="n">
+        <f aca="false">D34-C34</f>
         <v>0</v>
       </c>
       <c r="F34" s="10"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="9">
-        <f t="shared" si="1"/>
+      <c r="E35" s="9" t="n">
+        <f aca="false">D35-C35</f>
         <v>0</v>
       </c>
       <c r="F35" s="10"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="9">
-        <f t="shared" si="1"/>
+      <c r="E36" s="9" t="n">
+        <f aca="false">D36-C36</f>
         <v>0</v>
       </c>
       <c r="F36" s="10"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
-      <c r="E37" s="9">
-        <f t="shared" si="1"/>
+      <c r="E37" s="9" t="n">
+        <f aca="false">D37-C37</f>
         <v>0</v>
       </c>
       <c r="F37" s="10"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
-      <c r="E38" s="9">
-        <f t="shared" si="1"/>
+      <c r="E38" s="9" t="n">
+        <f aca="false">D38-C38</f>
         <v>0</v>
       </c>
       <c r="F38" s="10"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
-      <c r="E39" s="9">
-        <f t="shared" si="1"/>
+      <c r="E39" s="9" t="n">
+        <f aca="false">D39-C39</f>
         <v>0</v>
       </c>
       <c r="F39" s="10"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="9">
-        <f t="shared" si="1"/>
+      <c r="E40" s="9" t="n">
+        <f aca="false">D40-C40</f>
         <v>0</v>
       </c>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="9">
-        <f t="shared" si="1"/>
+      <c r="E41" s="9" t="n">
+        <f aca="false">D41-C41</f>
         <v>0</v>
       </c>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
-      <c r="E42" s="9">
-        <f t="shared" si="1"/>
+      <c r="E42" s="9" t="n">
+        <f aca="false">D42-C42</f>
         <v>0</v>
       </c>
       <c r="F42" s="10"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
-      <c r="E43" s="9">
-        <f t="shared" si="1"/>
+      <c r="E43" s="9" t="n">
+        <f aca="false">D43-C43</f>
         <v>0</v>
       </c>
       <c r="F43" s="10"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
-      <c r="E44" s="9">
-        <f t="shared" si="1"/>
+      <c r="E44" s="9" t="n">
+        <f aca="false">D44-C44</f>
         <v>0</v>
       </c>
       <c r="F44" s="10"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
-      <c r="E45" s="9">
-        <f t="shared" si="1"/>
+      <c r="E45" s="9" t="n">
+        <f aca="false">D45-C45</f>
         <v>0</v>
       </c>
       <c r="F45" s="10"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
-      <c r="E46" s="9">
-        <f t="shared" si="1"/>
+      <c r="E46" s="9" t="n">
+        <f aca="false">D46-C46</f>
         <v>0</v>
       </c>
       <c r="F46" s="10"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
-      <c r="E47" s="9">
-        <f t="shared" si="1"/>
+      <c r="E47" s="9" t="n">
+        <f aca="false">D47-C47</f>
         <v>0</v>
       </c>
       <c r="F47" s="10"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
-      <c r="E48" s="9">
-        <f t="shared" si="1"/>
+      <c r="E48" s="9" t="n">
+        <f aca="false">D48-C48</f>
         <v>0</v>
       </c>
       <c r="F48" s="10"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
-      <c r="E49" s="9">
-        <f t="shared" si="1"/>
+      <c r="E49" s="9" t="n">
+        <f aca="false">D49-C49</f>
         <v>0</v>
       </c>
       <c r="F49" s="10"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
-      <c r="E50" s="9">
-        <f t="shared" si="1"/>
+      <c r="E50" s="9" t="n">
+        <f aca="false">D50-C50</f>
         <v>0</v>
       </c>
       <c r="F50" s="10"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
-      <c r="E51" s="9">
-        <f t="shared" si="1"/>
+      <c r="E51" s="9" t="n">
+        <f aca="false">D51-C51</f>
         <v>0</v>
       </c>
       <c r="F51" s="10"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
-      <c r="E52" s="9">
-        <f t="shared" si="1"/>
+      <c r="E52" s="9" t="n">
+        <f aca="false">D52-C52</f>
         <v>0</v>
       </c>
       <c r="F52" s="10"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
-      <c r="E53" s="9">
-        <f t="shared" si="1"/>
+      <c r="E53" s="9" t="n">
+        <f aca="false">D53-C53</f>
         <v>0</v>
       </c>
       <c r="F53" s="10"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
-      <c r="E54" s="9">
-        <f t="shared" si="1"/>
+      <c r="E54" s="9" t="n">
+        <f aca="false">D54-C54</f>
         <v>0</v>
       </c>
       <c r="F54" s="10"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
-      <c r="E55" s="9">
-        <f t="shared" si="1"/>
+      <c r="E55" s="9" t="n">
+        <f aca="false">D55-C55</f>
         <v>0</v>
       </c>
       <c r="F55" s="10"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
-      <c r="E56" s="9">
-        <f t="shared" si="1"/>
+      <c r="E56" s="9" t="n">
+        <f aca="false">D56-C56</f>
         <v>0</v>
       </c>
       <c r="F56" s="10"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
-      <c r="E57" s="9">
-        <f t="shared" si="1"/>
+      <c r="E57" s="9" t="n">
+        <f aca="false">D57-C57</f>
         <v>0</v>
       </c>
       <c r="F57" s="10"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
-      <c r="E58" s="9">
-        <f t="shared" si="1"/>
+      <c r="E58" s="9" t="n">
+        <f aca="false">D58-C58</f>
         <v>0</v>
       </c>
       <c r="F58" s="10"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
-      <c r="E59" s="9">
-        <f t="shared" si="1"/>
+      <c r="E59" s="9" t="n">
+        <f aca="false">D59-C59</f>
         <v>0</v>
       </c>
       <c r="F59" s="10"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
-      <c r="E60" s="9">
-        <f t="shared" si="1"/>
+      <c r="E60" s="9" t="n">
+        <f aca="false">D60-C60</f>
         <v>0</v>
       </c>
       <c r="F60" s="10"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
-      <c r="E61" s="9">
-        <f t="shared" si="1"/>
+      <c r="E61" s="9" t="n">
+        <f aca="false">D61-C61</f>
         <v>0</v>
       </c>
       <c r="F61" s="10"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
-      <c r="E62" s="9">
-        <f t="shared" si="1"/>
+      <c r="E62" s="9" t="n">
+        <f aca="false">D62-C62</f>
         <v>0</v>
       </c>
       <c r="F62" s="10"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
-      <c r="E63" s="9">
-        <f t="shared" si="1"/>
+      <c r="E63" s="9" t="n">
+        <f aca="false">D63-C63</f>
         <v>0</v>
       </c>
       <c r="F63" s="10"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
-      <c r="E64" s="9">
-        <f t="shared" si="1"/>
+      <c r="E64" s="9" t="n">
+        <f aca="false">D64-C64</f>
         <v>0</v>
       </c>
       <c r="F64" s="10"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
-      <c r="E65" s="9">
-        <f t="shared" si="1"/>
+      <c r="E65" s="9" t="n">
+        <f aca="false">D65-C65</f>
         <v>0</v>
       </c>
       <c r="F65" s="10"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
-      <c r="E66" s="9">
-        <f t="shared" si="1"/>
+      <c r="E66" s="9" t="n">
+        <f aca="false">D66-C66</f>
         <v>0</v>
       </c>
       <c r="F66" s="10"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
-      <c r="E67" s="9">
-        <f t="shared" si="1"/>
+      <c r="E67" s="9" t="n">
+        <f aca="false">D67-C67</f>
         <v>0</v>
       </c>
       <c r="F67" s="10"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
-      <c r="E68" s="9">
-        <f t="shared" si="1"/>
+      <c r="E68" s="9" t="n">
+        <f aca="false">D68-C68</f>
         <v>0</v>
       </c>
       <c r="F68" s="10"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
-      <c r="E69" s="9">
-        <f t="shared" ref="E69:E132" si="2">D69-C69</f>
+      <c r="E69" s="9" t="n">
+        <f aca="false">D69-C69</f>
         <v>0</v>
       </c>
       <c r="F69" s="10"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
-      <c r="E70" s="9">
-        <f t="shared" si="2"/>
+      <c r="E70" s="9" t="n">
+        <f aca="false">D70-C70</f>
         <v>0</v>
       </c>
       <c r="F70" s="10"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
-      <c r="E71" s="9">
-        <f t="shared" si="2"/>
+      <c r="E71" s="9" t="n">
+        <f aca="false">D71-C71</f>
         <v>0</v>
       </c>
       <c r="F71" s="10"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
-      <c r="E72" s="9">
-        <f t="shared" si="2"/>
+      <c r="E72" s="9" t="n">
+        <f aca="false">D72-C72</f>
         <v>0</v>
       </c>
       <c r="F72" s="10"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
-      <c r="E73" s="9">
-        <f t="shared" si="2"/>
+      <c r="E73" s="9" t="n">
+        <f aca="false">D73-C73</f>
         <v>0</v>
       </c>
       <c r="F73" s="10"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
-      <c r="E74" s="9">
-        <f t="shared" si="2"/>
+      <c r="E74" s="9" t="n">
+        <f aca="false">D74-C74</f>
         <v>0</v>
       </c>
       <c r="F74" s="10"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
-      <c r="E75" s="9">
-        <f t="shared" si="2"/>
+      <c r="E75" s="9" t="n">
+        <f aca="false">D75-C75</f>
         <v>0</v>
       </c>
       <c r="F75" s="10"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
-      <c r="E76" s="9">
-        <f t="shared" si="2"/>
+      <c r="E76" s="9" t="n">
+        <f aca="false">D76-C76</f>
         <v>0</v>
       </c>
       <c r="F76" s="10"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
-      <c r="E77" s="9">
-        <f t="shared" si="2"/>
+      <c r="E77" s="9" t="n">
+        <f aca="false">D77-C77</f>
         <v>0</v>
       </c>
       <c r="F77" s="10"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
-      <c r="E78" s="9">
-        <f t="shared" si="2"/>
+      <c r="E78" s="9" t="n">
+        <f aca="false">D78-C78</f>
         <v>0</v>
       </c>
       <c r="F78" s="10"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
-      <c r="E79" s="9">
-        <f t="shared" si="2"/>
+      <c r="E79" s="9" t="n">
+        <f aca="false">D79-C79</f>
         <v>0</v>
       </c>
       <c r="F79" s="10"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
-      <c r="E80" s="9">
-        <f t="shared" si="2"/>
+      <c r="E80" s="9" t="n">
+        <f aca="false">D80-C80</f>
         <v>0</v>
       </c>
       <c r="F80" s="10"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
-      <c r="E81" s="9">
-        <f t="shared" si="2"/>
+      <c r="E81" s="9" t="n">
+        <f aca="false">D81-C81</f>
         <v>0</v>
       </c>
       <c r="F81" s="10"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
-      <c r="E82" s="9">
-        <f t="shared" si="2"/>
+      <c r="E82" s="9" t="n">
+        <f aca="false">D82-C82</f>
         <v>0</v>
       </c>
       <c r="F82" s="10"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
-      <c r="E83" s="9">
-        <f t="shared" si="2"/>
+      <c r="E83" s="9" t="n">
+        <f aca="false">D83-C83</f>
         <v>0</v>
       </c>
       <c r="F83" s="10"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
-      <c r="E84" s="9">
-        <f t="shared" si="2"/>
+      <c r="E84" s="9" t="n">
+        <f aca="false">D84-C84</f>
         <v>0</v>
       </c>
       <c r="F84" s="10"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
-      <c r="E85" s="9">
-        <f t="shared" si="2"/>
+      <c r="E85" s="9" t="n">
+        <f aca="false">D85-C85</f>
         <v>0</v>
       </c>
       <c r="F85" s="10"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
-      <c r="E86" s="9">
-        <f t="shared" si="2"/>
+      <c r="E86" s="9" t="n">
+        <f aca="false">D86-C86</f>
         <v>0</v>
       </c>
       <c r="F86" s="10"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
-      <c r="E87" s="9">
-        <f t="shared" si="2"/>
+      <c r="E87" s="9" t="n">
+        <f aca="false">D87-C87</f>
         <v>0</v>
       </c>
       <c r="F87" s="10"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
-      <c r="E88" s="9">
-        <f t="shared" si="2"/>
+      <c r="E88" s="9" t="n">
+        <f aca="false">D88-C88</f>
         <v>0</v>
       </c>
       <c r="F88" s="10"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
-      <c r="E89" s="9">
-        <f t="shared" si="2"/>
+      <c r="E89" s="9" t="n">
+        <f aca="false">D89-C89</f>
         <v>0</v>
       </c>
       <c r="F89" s="10"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
-      <c r="E90" s="9">
-        <f t="shared" si="2"/>
+      <c r="E90" s="9" t="n">
+        <f aca="false">D90-C90</f>
         <v>0</v>
       </c>
       <c r="F90" s="10"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
-      <c r="E91" s="9">
-        <f t="shared" si="2"/>
+      <c r="E91" s="9" t="n">
+        <f aca="false">D91-C91</f>
         <v>0</v>
       </c>
       <c r="F91" s="10"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
-      <c r="E92" s="9">
-        <f t="shared" si="2"/>
+      <c r="E92" s="9" t="n">
+        <f aca="false">D92-C92</f>
         <v>0</v>
       </c>
       <c r="F92" s="10"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
-      <c r="E93" s="9">
-        <f t="shared" si="2"/>
+      <c r="E93" s="9" t="n">
+        <f aca="false">D93-C93</f>
         <v>0</v>
       </c>
       <c r="F93" s="10"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
-      <c r="E94" s="9">
-        <f t="shared" si="2"/>
+      <c r="E94" s="9" t="n">
+        <f aca="false">D94-C94</f>
         <v>0</v>
       </c>
       <c r="F94" s="10"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
-      <c r="E95" s="9">
-        <f t="shared" si="2"/>
+      <c r="E95" s="9" t="n">
+        <f aca="false">D95-C95</f>
         <v>0</v>
       </c>
       <c r="F95" s="10"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
-      <c r="E96" s="9">
-        <f t="shared" si="2"/>
+      <c r="E96" s="9" t="n">
+        <f aca="false">D96-C96</f>
         <v>0</v>
       </c>
       <c r="F96" s="10"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
-      <c r="E97" s="9">
-        <f t="shared" si="2"/>
+      <c r="E97" s="9" t="n">
+        <f aca="false">D97-C97</f>
         <v>0</v>
       </c>
       <c r="F97" s="10"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
-      <c r="E98" s="9">
-        <f t="shared" si="2"/>
+      <c r="E98" s="9" t="n">
+        <f aca="false">D98-C98</f>
         <v>0</v>
       </c>
       <c r="F98" s="10"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
-      <c r="E99" s="9">
-        <f t="shared" si="2"/>
+      <c r="E99" s="9" t="n">
+        <f aca="false">D99-C99</f>
         <v>0</v>
       </c>
       <c r="F99" s="10"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
-      <c r="E100" s="9">
-        <f t="shared" si="2"/>
+      <c r="E100" s="9" t="n">
+        <f aca="false">D100-C100</f>
         <v>0</v>
       </c>
       <c r="F100" s="10"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
-      <c r="E101" s="9">
-        <f t="shared" si="2"/>
+      <c r="E101" s="9" t="n">
+        <f aca="false">D101-C101</f>
         <v>0</v>
       </c>
       <c r="F101" s="10"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
-      <c r="E102" s="9">
-        <f t="shared" si="2"/>
+      <c r="E102" s="9" t="n">
+        <f aca="false">D102-C102</f>
         <v>0</v>
       </c>
       <c r="F102" s="10"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
-      <c r="E103" s="9">
-        <f t="shared" si="2"/>
+      <c r="E103" s="9" t="n">
+        <f aca="false">D103-C103</f>
         <v>0</v>
       </c>
       <c r="F103" s="10"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
-      <c r="E104" s="9">
-        <f t="shared" si="2"/>
+      <c r="E104" s="9" t="n">
+        <f aca="false">D104-C104</f>
         <v>0</v>
       </c>
       <c r="F104" s="10"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
-      <c r="E105" s="9">
-        <f t="shared" si="2"/>
+      <c r="E105" s="9" t="n">
+        <f aca="false">D105-C105</f>
         <v>0</v>
       </c>
       <c r="F105" s="10"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
-      <c r="E106" s="9">
-        <f t="shared" si="2"/>
+      <c r="E106" s="9" t="n">
+        <f aca="false">D106-C106</f>
         <v>0</v>
       </c>
       <c r="F106" s="10"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
-      <c r="E107" s="9">
-        <f t="shared" si="2"/>
+      <c r="E107" s="9" t="n">
+        <f aca="false">D107-C107</f>
         <v>0</v>
       </c>
       <c r="F107" s="10"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
-      <c r="E108" s="9">
-        <f t="shared" si="2"/>
+      <c r="E108" s="9" t="n">
+        <f aca="false">D108-C108</f>
         <v>0</v>
       </c>
       <c r="F108" s="10"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
-      <c r="E109" s="9">
-        <f t="shared" si="2"/>
+      <c r="E109" s="9" t="n">
+        <f aca="false">D109-C109</f>
         <v>0</v>
       </c>
       <c r="F109" s="10"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
-      <c r="E110" s="9">
-        <f t="shared" si="2"/>
+      <c r="E110" s="9" t="n">
+        <f aca="false">D110-C110</f>
         <v>0</v>
       </c>
       <c r="F110" s="10"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
-      <c r="E111" s="9">
-        <f t="shared" si="2"/>
+      <c r="E111" s="9" t="n">
+        <f aca="false">D111-C111</f>
         <v>0</v>
       </c>
       <c r="F111" s="10"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
-      <c r="E112" s="9">
-        <f t="shared" si="2"/>
+      <c r="E112" s="9" t="n">
+        <f aca="false">D112-C112</f>
         <v>0</v>
       </c>
       <c r="F112" s="10"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
-      <c r="E113" s="9">
-        <f t="shared" si="2"/>
+      <c r="E113" s="9" t="n">
+        <f aca="false">D113-C113</f>
         <v>0</v>
       </c>
       <c r="F113" s="10"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
-      <c r="E114" s="9">
-        <f t="shared" si="2"/>
+      <c r="E114" s="9" t="n">
+        <f aca="false">D114-C114</f>
         <v>0</v>
       </c>
       <c r="F114" s="10"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
-      <c r="E115" s="9">
-        <f t="shared" si="2"/>
+      <c r="E115" s="9" t="n">
+        <f aca="false">D115-C115</f>
         <v>0</v>
       </c>
       <c r="F115" s="10"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
-      <c r="E116" s="9">
-        <f t="shared" si="2"/>
+      <c r="E116" s="9" t="n">
+        <f aca="false">D116-C116</f>
         <v>0</v>
       </c>
       <c r="F116" s="10"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
-      <c r="E117" s="9">
-        <f t="shared" si="2"/>
+      <c r="E117" s="9" t="n">
+        <f aca="false">D117-C117</f>
         <v>0</v>
       </c>
       <c r="F117" s="10"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
-      <c r="E118" s="9">
-        <f t="shared" si="2"/>
+      <c r="E118" s="9" t="n">
+        <f aca="false">D118-C118</f>
         <v>0</v>
       </c>
       <c r="F118" s="10"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
-      <c r="E119" s="9">
-        <f t="shared" si="2"/>
+      <c r="E119" s="9" t="n">
+        <f aca="false">D119-C119</f>
         <v>0</v>
       </c>
       <c r="F119" s="10"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
-      <c r="E120" s="9">
-        <f t="shared" si="2"/>
+      <c r="E120" s="9" t="n">
+        <f aca="false">D120-C120</f>
         <v>0</v>
       </c>
       <c r="F120" s="10"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
-      <c r="E121" s="9">
-        <f t="shared" si="2"/>
+      <c r="E121" s="9" t="n">
+        <f aca="false">D121-C121</f>
         <v>0</v>
       </c>
       <c r="F121" s="10"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
-      <c r="E122" s="9">
-        <f t="shared" si="2"/>
+      <c r="E122" s="9" t="n">
+        <f aca="false">D122-C122</f>
         <v>0</v>
       </c>
       <c r="F122" s="10"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
-      <c r="E123" s="9">
-        <f t="shared" si="2"/>
+      <c r="E123" s="9" t="n">
+        <f aca="false">D123-C123</f>
         <v>0</v>
       </c>
       <c r="F123" s="10"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
-      <c r="E124" s="9">
-        <f t="shared" si="2"/>
+      <c r="E124" s="9" t="n">
+        <f aca="false">D124-C124</f>
         <v>0</v>
       </c>
       <c r="F124" s="10"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
-      <c r="E125" s="9">
-        <f t="shared" si="2"/>
+      <c r="E125" s="9" t="n">
+        <f aca="false">D125-C125</f>
         <v>0</v>
       </c>
       <c r="F125" s="10"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
-      <c r="E126" s="9">
-        <f t="shared" si="2"/>
+      <c r="E126" s="9" t="n">
+        <f aca="false">D126-C126</f>
         <v>0</v>
       </c>
       <c r="F126" s="10"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="7"/>
       <c r="B127" s="7"/>
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
-      <c r="E127" s="9">
-        <f t="shared" si="2"/>
+      <c r="E127" s="9" t="n">
+        <f aca="false">D127-C127</f>
         <v>0</v>
       </c>
       <c r="F127" s="10"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="7"/>
       <c r="B128" s="7"/>
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
-      <c r="E128" s="9">
-        <f t="shared" si="2"/>
+      <c r="E128" s="9" t="n">
+        <f aca="false">D128-C128</f>
         <v>0</v>
       </c>
       <c r="F128" s="10"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="7"/>
       <c r="D129" s="7"/>
-      <c r="E129" s="9">
-        <f t="shared" si="2"/>
+      <c r="E129" s="9" t="n">
+        <f aca="false">D129-C129</f>
         <v>0</v>
       </c>
       <c r="F129" s="10"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
       <c r="D130" s="7"/>
-      <c r="E130" s="9">
-        <f t="shared" si="2"/>
+      <c r="E130" s="9" t="n">
+        <f aca="false">D130-C130</f>
         <v>0</v>
       </c>
       <c r="F130" s="10"/>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="7"/>
       <c r="D131" s="7"/>
-      <c r="E131" s="9">
-        <f t="shared" si="2"/>
+      <c r="E131" s="9" t="n">
+        <f aca="false">D131-C131</f>
         <v>0</v>
       </c>
       <c r="F131" s="10"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
-      <c r="E132" s="9">
-        <f t="shared" si="2"/>
+      <c r="E132" s="9" t="n">
+        <f aca="false">D132-C132</f>
         <v>0</v>
       </c>
       <c r="F132" s="10"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="7"/>
       <c r="D133" s="7"/>
-      <c r="E133" s="9">
-        <f t="shared" ref="E133:E196" si="3">D133-C133</f>
+      <c r="E133" s="9" t="n">
+        <f aca="false">D133-C133</f>
         <v>0</v>
       </c>
       <c r="F133" s="10"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
       <c r="D134" s="7"/>
-      <c r="E134" s="9">
-        <f t="shared" si="3"/>
+      <c r="E134" s="9" t="n">
+        <f aca="false">D134-C134</f>
         <v>0</v>
       </c>
       <c r="F134" s="10"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
       <c r="D135" s="7"/>
-      <c r="E135" s="9">
-        <f t="shared" si="3"/>
+      <c r="E135" s="9" t="n">
+        <f aca="false">D135-C135</f>
         <v>0</v>
       </c>
       <c r="F135" s="10"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
       <c r="D136" s="7"/>
-      <c r="E136" s="9">
-        <f t="shared" si="3"/>
+      <c r="E136" s="9" t="n">
+        <f aca="false">D136-C136</f>
         <v>0</v>
       </c>
       <c r="F136" s="10"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
       <c r="C137" s="7"/>
       <c r="D137" s="7"/>
-      <c r="E137" s="9">
-        <f t="shared" si="3"/>
+      <c r="E137" s="9" t="n">
+        <f aca="false">D137-C137</f>
         <v>0</v>
       </c>
       <c r="F137" s="10"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
-      <c r="E138" s="9">
-        <f t="shared" si="3"/>
+      <c r="E138" s="9" t="n">
+        <f aca="false">D138-C138</f>
         <v>0</v>
       </c>
       <c r="F138" s="10"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
       <c r="D139" s="7"/>
-      <c r="E139" s="9">
-        <f t="shared" si="3"/>
+      <c r="E139" s="9" t="n">
+        <f aca="false">D139-C139</f>
         <v>0</v>
       </c>
       <c r="F139" s="10"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
-      <c r="E140" s="9">
-        <f t="shared" si="3"/>
+      <c r="E140" s="9" t="n">
+        <f aca="false">D140-C140</f>
         <v>0</v>
       </c>
       <c r="F140" s="10"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
       <c r="D141" s="7"/>
-      <c r="E141" s="9">
-        <f t="shared" si="3"/>
+      <c r="E141" s="9" t="n">
+        <f aca="false">D141-C141</f>
         <v>0</v>
       </c>
       <c r="F141" s="10"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="7"/>
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
-      <c r="E142" s="9">
-        <f t="shared" si="3"/>
+      <c r="E142" s="9" t="n">
+        <f aca="false">D142-C142</f>
         <v>0</v>
       </c>
       <c r="F142" s="10"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="7"/>
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
       <c r="D143" s="7"/>
-      <c r="E143" s="9">
-        <f t="shared" si="3"/>
+      <c r="E143" s="9" t="n">
+        <f aca="false">D143-C143</f>
         <v>0</v>
       </c>
       <c r="F143" s="10"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="7"/>
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
-      <c r="E144" s="9">
-        <f t="shared" si="3"/>
+      <c r="E144" s="9" t="n">
+        <f aca="false">D144-C144</f>
         <v>0</v>
       </c>
       <c r="F144" s="10"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
       <c r="D145" s="7"/>
-      <c r="E145" s="9">
-        <f t="shared" si="3"/>
+      <c r="E145" s="9" t="n">
+        <f aca="false">D145-C145</f>
         <v>0</v>
       </c>
       <c r="F145" s="10"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="7"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
-      <c r="E146" s="9">
-        <f t="shared" si="3"/>
+      <c r="E146" s="9" t="n">
+        <f aca="false">D146-C146</f>
         <v>0</v>
       </c>
       <c r="F146" s="10"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="7"/>
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
-      <c r="E147" s="9">
-        <f t="shared" si="3"/>
+      <c r="E147" s="9" t="n">
+        <f aca="false">D147-C147</f>
         <v>0</v>
       </c>
       <c r="F147" s="10"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="7"/>
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
-      <c r="E148" s="9">
-        <f t="shared" si="3"/>
+      <c r="E148" s="9" t="n">
+        <f aca="false">D148-C148</f>
         <v>0</v>
       </c>
       <c r="F148" s="10"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="7"/>
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
       <c r="D149" s="7"/>
-      <c r="E149" s="9">
-        <f t="shared" si="3"/>
+      <c r="E149" s="9" t="n">
+        <f aca="false">D149-C149</f>
         <v>0</v>
       </c>
       <c r="F149" s="10"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="7"/>
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
       <c r="D150" s="7"/>
-      <c r="E150" s="9">
-        <f t="shared" si="3"/>
+      <c r="E150" s="9" t="n">
+        <f aca="false">D150-C150</f>
         <v>0</v>
       </c>
       <c r="F150" s="10"/>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="7"/>
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
       <c r="D151" s="7"/>
-      <c r="E151" s="9">
-        <f t="shared" si="3"/>
+      <c r="E151" s="9" t="n">
+        <f aca="false">D151-C151</f>
         <v>0</v>
       </c>
       <c r="F151" s="10"/>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="7"/>
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
-      <c r="E152" s="9">
-        <f t="shared" si="3"/>
+      <c r="E152" s="9" t="n">
+        <f aca="false">D152-C152</f>
         <v>0</v>
       </c>
       <c r="F152" s="10"/>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="7"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
-      <c r="E153" s="9">
-        <f t="shared" si="3"/>
+      <c r="E153" s="9" t="n">
+        <f aca="false">D153-C153</f>
         <v>0</v>
       </c>
       <c r="F153" s="10"/>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="7"/>
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
-      <c r="E154" s="9">
-        <f t="shared" si="3"/>
+      <c r="E154" s="9" t="n">
+        <f aca="false">D154-C154</f>
         <v>0</v>
       </c>
       <c r="F154" s="10"/>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="7"/>
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
       <c r="D155" s="7"/>
-      <c r="E155" s="9">
-        <f t="shared" si="3"/>
+      <c r="E155" s="9" t="n">
+        <f aca="false">D155-C155</f>
         <v>0</v>
       </c>
       <c r="F155" s="10"/>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="7"/>
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
       <c r="D156" s="7"/>
-      <c r="E156" s="9">
-        <f t="shared" si="3"/>
+      <c r="E156" s="9" t="n">
+        <f aca="false">D156-C156</f>
         <v>0</v>
       </c>
       <c r="F156" s="10"/>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="7"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
       <c r="D157" s="7"/>
-      <c r="E157" s="9">
-        <f t="shared" si="3"/>
+      <c r="E157" s="9" t="n">
+        <f aca="false">D157-C157</f>
         <v>0</v>
       </c>
       <c r="F157" s="10"/>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="7"/>
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
-      <c r="E158" s="9">
-        <f t="shared" si="3"/>
+      <c r="E158" s="9" t="n">
+        <f aca="false">D158-C158</f>
         <v>0</v>
       </c>
       <c r="F158" s="10"/>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="7"/>
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
-      <c r="E159" s="9">
-        <f t="shared" si="3"/>
+      <c r="E159" s="9" t="n">
+        <f aca="false">D159-C159</f>
         <v>0</v>
       </c>
       <c r="F159" s="10"/>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="7"/>
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
       <c r="D160" s="7"/>
-      <c r="E160" s="9">
-        <f t="shared" si="3"/>
+      <c r="E160" s="9" t="n">
+        <f aca="false">D160-C160</f>
         <v>0</v>
       </c>
       <c r="F160" s="10"/>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="7"/>
       <c r="B161" s="7"/>
       <c r="C161" s="7"/>
       <c r="D161" s="7"/>
-      <c r="E161" s="9">
-        <f t="shared" si="3"/>
+      <c r="E161" s="9" t="n">
+        <f aca="false">D161-C161</f>
         <v>0</v>
       </c>
       <c r="F161" s="10"/>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
       <c r="D162" s="7"/>
-      <c r="E162" s="9">
-        <f t="shared" si="3"/>
+      <c r="E162" s="9" t="n">
+        <f aca="false">D162-C162</f>
         <v>0</v>
       </c>
       <c r="F162" s="10"/>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="7"/>
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
       <c r="D163" s="7"/>
-      <c r="E163" s="9">
-        <f t="shared" si="3"/>
+      <c r="E163" s="9" t="n">
+        <f aca="false">D163-C163</f>
         <v>0</v>
       </c>
       <c r="F163" s="10"/>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
-      <c r="E164" s="9">
-        <f t="shared" si="3"/>
+      <c r="E164" s="9" t="n">
+        <f aca="false">D164-C164</f>
         <v>0</v>
       </c>
       <c r="F164" s="10"/>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="7"/>
       <c r="B165" s="7"/>
       <c r="C165" s="7"/>
       <c r="D165" s="7"/>
-      <c r="E165" s="9">
-        <f t="shared" si="3"/>
+      <c r="E165" s="9" t="n">
+        <f aca="false">D165-C165</f>
         <v>0</v>
       </c>
       <c r="F165" s="10"/>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
       <c r="D166" s="7"/>
-      <c r="E166" s="9">
-        <f t="shared" si="3"/>
+      <c r="E166" s="9" t="n">
+        <f aca="false">D166-C166</f>
         <v>0</v>
       </c>
       <c r="F166" s="10"/>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="7"/>
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
       <c r="D167" s="7"/>
-      <c r="E167" s="9">
-        <f t="shared" si="3"/>
+      <c r="E167" s="9" t="n">
+        <f aca="false">D167-C167</f>
         <v>0</v>
       </c>
       <c r="F167" s="10"/>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
       <c r="D168" s="7"/>
-      <c r="E168" s="9">
-        <f t="shared" si="3"/>
+      <c r="E168" s="9" t="n">
+        <f aca="false">D168-C168</f>
         <v>0</v>
       </c>
       <c r="F168" s="10"/>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="7"/>
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
       <c r="D169" s="7"/>
-      <c r="E169" s="9">
-        <f t="shared" si="3"/>
+      <c r="E169" s="9" t="n">
+        <f aca="false">D169-C169</f>
         <v>0</v>
       </c>
       <c r="F169" s="10"/>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
       <c r="D170" s="7"/>
-      <c r="E170" s="9">
-        <f t="shared" si="3"/>
+      <c r="E170" s="9" t="n">
+        <f aca="false">D170-C170</f>
         <v>0</v>
       </c>
       <c r="F170" s="10"/>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="7"/>
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
       <c r="D171" s="7"/>
-      <c r="E171" s="9">
-        <f t="shared" si="3"/>
+      <c r="E171" s="9" t="n">
+        <f aca="false">D171-C171</f>
         <v>0</v>
       </c>
       <c r="F171" s="10"/>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
       <c r="D172" s="7"/>
-      <c r="E172" s="9">
-        <f t="shared" si="3"/>
+      <c r="E172" s="9" t="n">
+        <f aca="false">D172-C172</f>
         <v>0</v>
       </c>
       <c r="F172" s="10"/>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="7"/>
       <c r="B173" s="7"/>
       <c r="C173" s="7"/>
       <c r="D173" s="7"/>
-      <c r="E173" s="9">
-        <f t="shared" si="3"/>
+      <c r="E173" s="9" t="n">
+        <f aca="false">D173-C173</f>
         <v>0</v>
       </c>
       <c r="F173" s="10"/>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="7"/>
       <c r="B174" s="7"/>
       <c r="C174" s="7"/>
       <c r="D174" s="7"/>
-      <c r="E174" s="9">
-        <f t="shared" si="3"/>
+      <c r="E174" s="9" t="n">
+        <f aca="false">D174-C174</f>
         <v>0</v>
       </c>
       <c r="F174" s="10"/>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="7"/>
       <c r="B175" s="7"/>
       <c r="C175" s="7"/>
       <c r="D175" s="7"/>
-      <c r="E175" s="9">
-        <f t="shared" si="3"/>
+      <c r="E175" s="9" t="n">
+        <f aca="false">D175-C175</f>
         <v>0</v>
       </c>
       <c r="F175" s="10"/>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="7"/>
       <c r="B176" s="7"/>
       <c r="C176" s="7"/>
       <c r="D176" s="7"/>
-      <c r="E176" s="9">
-        <f t="shared" si="3"/>
+      <c r="E176" s="9" t="n">
+        <f aca="false">D176-C176</f>
         <v>0</v>
       </c>
       <c r="F176" s="10"/>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="7"/>
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
       <c r="D177" s="7"/>
-      <c r="E177" s="9">
-        <f t="shared" si="3"/>
+      <c r="E177" s="9" t="n">
+        <f aca="false">D177-C177</f>
         <v>0</v>
       </c>
       <c r="F177" s="10"/>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="7"/>
       <c r="B178" s="7"/>
       <c r="C178" s="7"/>
       <c r="D178" s="7"/>
-      <c r="E178" s="9">
-        <f t="shared" si="3"/>
+      <c r="E178" s="9" t="n">
+        <f aca="false">D178-C178</f>
         <v>0</v>
       </c>
       <c r="F178" s="10"/>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="7"/>
       <c r="B179" s="7"/>
       <c r="C179" s="7"/>
       <c r="D179" s="7"/>
-      <c r="E179" s="9">
-        <f t="shared" si="3"/>
+      <c r="E179" s="9" t="n">
+        <f aca="false">D179-C179</f>
         <v>0</v>
       </c>
       <c r="F179" s="10"/>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="7"/>
       <c r="B180" s="7"/>
       <c r="C180" s="7"/>
       <c r="D180" s="7"/>
-      <c r="E180" s="9">
-        <f t="shared" si="3"/>
+      <c r="E180" s="9" t="n">
+        <f aca="false">D180-C180</f>
         <v>0</v>
       </c>
       <c r="F180" s="10"/>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="7"/>
       <c r="B181" s="7"/>
       <c r="C181" s="7"/>
       <c r="D181" s="7"/>
-      <c r="E181" s="9">
-        <f t="shared" si="3"/>
+      <c r="E181" s="9" t="n">
+        <f aca="false">D181-C181</f>
         <v>0</v>
       </c>
       <c r="F181" s="10"/>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="7"/>
       <c r="B182" s="7"/>
       <c r="C182" s="7"/>
       <c r="D182" s="7"/>
-      <c r="E182" s="9">
-        <f t="shared" si="3"/>
+      <c r="E182" s="9" t="n">
+        <f aca="false">D182-C182</f>
         <v>0</v>
       </c>
       <c r="F182" s="10"/>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="7"/>
       <c r="B183" s="7"/>
       <c r="C183" s="7"/>
       <c r="D183" s="7"/>
-      <c r="E183" s="9">
-        <f t="shared" si="3"/>
+      <c r="E183" s="9" t="n">
+        <f aca="false">D183-C183</f>
         <v>0</v>
       </c>
       <c r="F183" s="10"/>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="7"/>
       <c r="B184" s="7"/>
       <c r="C184" s="7"/>
       <c r="D184" s="7"/>
-      <c r="E184" s="9">
-        <f t="shared" si="3"/>
+      <c r="E184" s="9" t="n">
+        <f aca="false">D184-C184</f>
         <v>0</v>
       </c>
       <c r="F184" s="10"/>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="7"/>
       <c r="B185" s="7"/>
       <c r="C185" s="7"/>
       <c r="D185" s="7"/>
-      <c r="E185" s="9">
-        <f t="shared" si="3"/>
+      <c r="E185" s="9" t="n">
+        <f aca="false">D185-C185</f>
         <v>0</v>
       </c>
       <c r="F185" s="10"/>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="7"/>
       <c r="B186" s="7"/>
       <c r="C186" s="7"/>
       <c r="D186" s="7"/>
-      <c r="E186" s="9">
-        <f t="shared" si="3"/>
+      <c r="E186" s="9" t="n">
+        <f aca="false">D186-C186</f>
         <v>0</v>
       </c>
       <c r="F186" s="10"/>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="7"/>
       <c r="B187" s="7"/>
       <c r="C187" s="7"/>
       <c r="D187" s="7"/>
-      <c r="E187" s="9">
-        <f t="shared" si="3"/>
+      <c r="E187" s="9" t="n">
+        <f aca="false">D187-C187</f>
         <v>0</v>
       </c>
       <c r="F187" s="10"/>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="7"/>
       <c r="B188" s="7"/>
       <c r="C188" s="7"/>
       <c r="D188" s="7"/>
-      <c r="E188" s="9">
-        <f t="shared" si="3"/>
+      <c r="E188" s="9" t="n">
+        <f aca="false">D188-C188</f>
         <v>0</v>
       </c>
       <c r="F188" s="10"/>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="7"/>
       <c r="B189" s="7"/>
       <c r="C189" s="7"/>
       <c r="D189" s="7"/>
-      <c r="E189" s="9">
-        <f t="shared" si="3"/>
+      <c r="E189" s="9" t="n">
+        <f aca="false">D189-C189</f>
         <v>0</v>
       </c>
       <c r="F189" s="10"/>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="7"/>
       <c r="B190" s="7"/>
       <c r="C190" s="7"/>
       <c r="D190" s="7"/>
-      <c r="E190" s="9">
-        <f t="shared" si="3"/>
+      <c r="E190" s="9" t="n">
+        <f aca="false">D190-C190</f>
         <v>0</v>
       </c>
       <c r="F190" s="10"/>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="7"/>
       <c r="B191" s="7"/>
       <c r="C191" s="7"/>
       <c r="D191" s="7"/>
-      <c r="E191" s="9">
-        <f t="shared" si="3"/>
+      <c r="E191" s="9" t="n">
+        <f aca="false">D191-C191</f>
         <v>0</v>
       </c>
       <c r="F191" s="10"/>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="7"/>
       <c r="B192" s="7"/>
       <c r="C192" s="7"/>
       <c r="D192" s="7"/>
-      <c r="E192" s="9">
-        <f t="shared" si="3"/>
+      <c r="E192" s="9" t="n">
+        <f aca="false">D192-C192</f>
         <v>0</v>
       </c>
       <c r="F192" s="10"/>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="7"/>
       <c r="B193" s="7"/>
       <c r="C193" s="7"/>
       <c r="D193" s="7"/>
-      <c r="E193" s="9">
-        <f t="shared" si="3"/>
+      <c r="E193" s="9" t="n">
+        <f aca="false">D193-C193</f>
         <v>0</v>
       </c>
       <c r="F193" s="10"/>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="7"/>
       <c r="B194" s="7"/>
       <c r="C194" s="7"/>
       <c r="D194" s="7"/>
-      <c r="E194" s="9">
-        <f t="shared" si="3"/>
+      <c r="E194" s="9" t="n">
+        <f aca="false">D194-C194</f>
         <v>0</v>
       </c>
       <c r="F194" s="10"/>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="7"/>
       <c r="B195" s="7"/>
       <c r="C195" s="7"/>
       <c r="D195" s="7"/>
-      <c r="E195" s="9">
-        <f t="shared" si="3"/>
+      <c r="E195" s="9" t="n">
+        <f aca="false">D195-C195</f>
         <v>0</v>
       </c>
       <c r="F195" s="10"/>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="7"/>
       <c r="B196" s="7"/>
       <c r="C196" s="7"/>
       <c r="D196" s="7"/>
-      <c r="E196" s="9">
-        <f t="shared" si="3"/>
+      <c r="E196" s="9" t="n">
+        <f aca="false">D196-C196</f>
         <v>0</v>
       </c>
       <c r="F196" s="10"/>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="7"/>
       <c r="B197" s="7"/>
       <c r="C197" s="7"/>
       <c r="D197" s="7"/>
-      <c r="E197" s="9">
-        <f t="shared" ref="E197:E199" si="4">D197-C197</f>
+      <c r="E197" s="9" t="n">
+        <f aca="false">D197-C197</f>
         <v>0</v>
       </c>
       <c r="F197" s="10"/>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="7"/>
       <c r="B198" s="7"/>
       <c r="C198" s="7"/>
       <c r="D198" s="7"/>
-      <c r="E198" s="9">
-        <f t="shared" si="4"/>
+      <c r="E198" s="9" t="n">
+        <f aca="false">D198-C198</f>
         <v>0</v>
       </c>
       <c r="F198" s="10"/>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="7"/>
       <c r="B199" s="7"/>
       <c r="C199" s="7"/>
       <c r="D199" s="7"/>
-      <c r="E199" s="9">
-        <f t="shared" si="4"/>
+      <c r="E199" s="9" t="n">
+        <f aca="false">D199-C199</f>
         <v>0</v>
       </c>
       <c r="F199" s="10"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating Timesheet from yesterday's work
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/TimeReport_CarterKreis.xlsx
+++ b/Documentation/TimeSheets/TimeReport_CarterKreis.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\plant-partner\Documentation\TimeSheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65536F9-35E9-443C-97C6-06A1E119B1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -20,102 +36,101 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
-    <t xml:space="preserve">Name:</t>
+    <t>Name:</t>
   </si>
   <si>
-    <t xml:space="preserve">Carter Kreis</t>
+    <t>Carter Kreis</t>
   </si>
   <si>
-    <t xml:space="preserve">Total Time:</t>
+    <t>Total Time:</t>
   </si>
   <si>
-    <t xml:space="preserve">Date:</t>
+    <t>Date:</t>
   </si>
   <si>
-    <t xml:space="preserve">General Category:</t>
+    <t>General Category:</t>
   </si>
   <si>
-    <t xml:space="preserve">Starting Time:</t>
+    <t>Starting Time:</t>
   </si>
   <si>
-    <t xml:space="preserve">Ending  Time:</t>
+    <t>Ending  Time:</t>
   </si>
   <si>
-    <t xml:space="preserve">Calculated Time Worked:</t>
+    <t>Calculated Time Worked:</t>
   </si>
   <si>
-    <t xml:space="preserve">Description:</t>
+    <t>Description:</t>
   </si>
   <si>
-    <t xml:space="preserve">Design Draft</t>
+    <t>Design Draft</t>
   </si>
   <si>
-    <t xml:space="preserve">Sat down with group after class to define project and  talk through all of Design Draft points (Deliverables, Requirements, Division of work, ect.)</t>
+    <t>Sat down with group after class to define project and  talk through all of Design Draft points (Deliverables, Requirements, Division of work, ect.)</t>
   </si>
   <si>
-    <t xml:space="preserve">Check-in</t>
+    <t>Check-in</t>
   </si>
   <si>
-    <t xml:space="preserve">Check-in 1: Met with group &amp; Tyler. Discussed our design draft, and asked questions regarding design plan and material buying</t>
+    <t>Check-in 1: Met with group &amp; Tyler. Discussed our design draft, and asked questions regarding design plan and material buying</t>
   </si>
   <si>
-    <t xml:space="preserve">Project Organization</t>
+    <t>Project Organization</t>
   </si>
   <si>
-    <t xml:space="preserve">Researched and implemented Github webhook which sends all updates from Github to Discord channel named github-updates</t>
+    <t>Researched and implemented Github webhook which sends all updates from Github to Discord channel named github-updates</t>
   </si>
   <si>
     <t xml:space="preserve">Check-in 2: Met with group &amp; Tyler. Reviewed out submitted design draft, discussed adding more hardware specification, and discussed with  group members to start buying materials and beginning research </t>
   </si>
   <si>
-    <t xml:space="preserve">Check-in 3: Met with group &amp; Tyler. Planned out pre-alpha build documentation, materials list, and basic codebase structure. I will be working on PCB Design and physical materials for prototypes</t>
+    <t>Check-in 3: Met with group &amp; Tyler. Planned out pre-alpha build documentation, materials list, and basic codebase structure. I will be working on PCB Design and physical materials for prototypes</t>
   </si>
   <si>
-    <t xml:space="preserve">Pre-Alpha Build</t>
+    <t>Pre-Alpha Build</t>
   </si>
   <si>
-    <t xml:space="preserve">Researched and begun setup of ESP-IDF through its VS Code extension</t>
+    <t>Researched and begun setup of ESP-IDF through its VS Code extension</t>
   </si>
   <si>
-    <t xml:space="preserve">Setup ESP-IDF extension in VS Code. Attempted Hello World example code but my laptop is not detecting ESP32 as a COM Port. We also continued to plan Pre-Alpha Build goal</t>
+    <t>Setup ESP-IDF extension in VS Code. Attempted Hello World example code but my laptop is not detecting ESP32 as a COM Port. We also continued to plan Pre-Alpha Build goal</t>
   </si>
   <si>
-    <t xml:space="preserve">Repeated issues with recursively cloning the submodule esp-idf. Cloning into the submodule itself took 10-12 minutes and the first two times some of the directories failed to clone on time.</t>
+    <t>Repeated issues with recursively cloning the submodule esp-idf. Cloning into the submodule itself took 10-12 minutes and the first two times some of the directories failed to clone on time.</t>
   </si>
   <si>
-    <t xml:space="preserve">Finally got the ESP-IDF to flash ESP32 after switching to my Ubuntu OS. Proceeded to research and write the code to turn on external GPIO LED that is wired on breadboard and on-board LED. Also helped containerize, clean-up, and comment overall code for Pre-Alpha Build</t>
+    <t>Finally got the ESP-IDF to flash ESP32 after switching to my Ubuntu OS. Proceeded to research and write the code to turn on external GPIO LED that is wired on breadboard and on-board LED. Also helped containerize, clean-up, and comment overall code for Pre-Alpha Build</t>
   </si>
   <si>
-    <t xml:space="preserve">Design Prototype</t>
+    <t>Design Prototype</t>
   </si>
   <si>
-    <t xml:space="preserve">Worked on trying to get the specific ESP-32 model by analyzing the ESP32 info structs. I also got ESP-IDF working on Windows which needed some drivers uninstalled then proper ones re-installed</t>
+    <t>Worked on trying to get the specific ESP-32 model by analyzing the ESP32 info structs. I also got ESP-IDF working on Windows which needed some drivers uninstalled then proper ones re-installed</t>
   </si>
   <si>
-    <t xml:space="preserve">Setup KiCad for PCB Design. Throughout this week and the next, I will figure out specific footprints for out sensors and design the PCB Schematic and then PCB design</t>
+    <t>Setup KiCad for PCB Design. Throughout this week and the next, I will figure out specific footprints for out sensors and design the PCB Schematic and then PCB design</t>
   </si>
   <si>
-    <t xml:space="preserve">Searched for and found my Infinity Stones (the schematics for each sensor for our PCB). Now that I gathered the schematics, I can start designing the PCB layout and how it will fit into our overall project and Design Prototype</t>
+    <t>Searched for and found my Infinity Stones (the schematics for each sensor for our PCB). Now that I gathered the schematics, I can start designing the PCB layout and how it will fit into our overall project and Design Prototype</t>
   </si>
   <si>
     <t xml:space="preserve">Finished PCB Schematic for Buck Converter and now working on RS-485 Transceiver Schematic. </t>
+  </si>
+  <si>
+    <t>Worked on UART driver code which includes an init, read, and write functions for standard UART modules and also a skeleton for RS-485 Half-duplex UART communication with the same three main functions (init, read, write)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[h]:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="167" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="168" formatCode="h:mm:ss"/>
-    <numFmt numFmtId="169" formatCode="hh:mm\ AM/PM"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="165" formatCode="hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,22 +139,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -156,7 +156,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.7999"/>
+        <fgColor theme="4" tint="0.79989013336588644"/>
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
@@ -174,128 +174,75 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="18" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="21" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -354,60 +301,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0e2841"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e8e8e8"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="e97132"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196b24"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0f9ed5"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="a02b93"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4ea72e"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607d"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -439,7 +402,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -463,7 +426,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -523,37 +486,36 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="244.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="1" width="8.86"/>
+    <col min="1" max="1" width="10.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24" style="1" customWidth="1"/>
+    <col min="6" max="6" width="244.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -563,13 +525,13 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="n">
-        <f aca="false">SUM(E4:E199)</f>
-        <v>1.08888888888889</v>
+      <c r="E1" s="4">
+        <f>SUM(E4:E199)</f>
+        <v>1.1930555555555555</v>
       </c>
       <c r="F1" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -589,2299 +551,2304 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>45933</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="n">
-        <v>0.470138888888889</v>
-      </c>
-      <c r="D4" s="8" t="n">
-        <v>0.610416666666667</v>
-      </c>
-      <c r="E4" s="9" t="n">
-        <f aca="false">D4-C4</f>
-        <v>0.140277777777778</v>
+      <c r="C4" s="8">
+        <v>0.47013888888888899</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.61041666666666705</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" ref="E4:E35" si="0">D4-C4</f>
+        <v>0.14027777777777806</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="n">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>45936</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8" t="n">
+      <c r="C5" s="8">
         <v>0.625</v>
       </c>
-      <c r="D5" s="8" t="n">
-        <v>0.647222222222222</v>
-      </c>
-      <c r="E5" s="9" t="n">
-        <f aca="false">D5-C5</f>
-        <v>0.0222222222222222</v>
+      <c r="D5" s="8">
+        <v>0.64722222222222203</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="0"/>
+        <v>2.2222222222222032E-2</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="n">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
         <v>45942</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="13" t="n">
-        <v>0.803472222222222</v>
-      </c>
-      <c r="D6" s="13" t="n">
-        <v>0.833333333333333</v>
-      </c>
-      <c r="E6" s="14" t="n">
-        <f aca="false">D6-C6</f>
-        <v>0.0298611111111111</v>
+      <c r="C6" s="13">
+        <v>0.80347222222222203</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" si="0"/>
+        <v>2.9861111111111005E-2</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="n">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>45944</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8" t="n">
-        <v>0.472222222222222</v>
-      </c>
-      <c r="D7" s="8" t="n">
-        <v>0.49375</v>
-      </c>
-      <c r="E7" s="9" t="n">
-        <f aca="false">D7-C7</f>
-        <v>0.0215277777777778</v>
+      <c r="C7" s="8">
+        <v>0.47222222222222199</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.49375000000000002</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="0"/>
+        <v>2.1527777777778034E-2</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="n">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>45950</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="8" t="n">
+      <c r="C8" s="8">
         <v>0.625</v>
       </c>
-      <c r="D8" s="8" t="n">
-        <v>0.647222222222222</v>
-      </c>
-      <c r="E8" s="9" t="n">
-        <f aca="false">D8-C8</f>
-        <v>0.0222222222222222</v>
+      <c r="D8" s="8">
+        <v>0.64722222222222203</v>
+      </c>
+      <c r="E8" s="9">
+        <f t="shared" si="0"/>
+        <v>2.2222222222222032E-2</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="n">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>45950</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8" t="n">
+      <c r="C9" s="8">
         <v>0.90625</v>
       </c>
-      <c r="D9" s="8" t="n">
-        <v>0.927083333333333</v>
-      </c>
-      <c r="E9" s="9" t="n">
-        <f aca="false">D9-C9</f>
-        <v>0.0208333333333333</v>
+      <c r="D9" s="8">
+        <v>0.92708333333333304</v>
+      </c>
+      <c r="E9" s="9">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333037E-2</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="n">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>45954</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="8" t="n">
-        <v>0.604166666666667</v>
-      </c>
-      <c r="D10" s="8" t="n">
-        <v>0.670138888888889</v>
-      </c>
-      <c r="E10" s="9" t="n">
-        <f aca="false">D10-C10</f>
-        <v>0.0659722222222222</v>
+      <c r="C10" s="8">
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.67013888888888895</v>
+      </c>
+      <c r="E10" s="9">
+        <f t="shared" si="0"/>
+        <v>6.5972222222221988E-2</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="n">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>45954</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="8" t="n">
-        <v>0.802083333333333</v>
-      </c>
-      <c r="D11" s="8" t="n">
-        <v>0.873611111111111</v>
-      </c>
-      <c r="E11" s="9" t="n">
-        <f aca="false">D11-C11</f>
-        <v>0.0715277777777778</v>
+      <c r="C11" s="8">
+        <v>0.80208333333333304</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.87361111111111101</v>
+      </c>
+      <c r="E11" s="9">
+        <f t="shared" si="0"/>
+        <v>7.1527777777777968E-2</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="n">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <v>45955</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="8" t="n">
-        <v>0.420138888888889</v>
-      </c>
-      <c r="D12" s="8" t="n">
-        <v>0.7375</v>
-      </c>
-      <c r="E12" s="9" t="n">
-        <f aca="false">D12-C12</f>
-        <v>0.317361111111111</v>
+      <c r="C12" s="8">
+        <v>0.42013888888888901</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="E12" s="9">
+        <f t="shared" si="0"/>
+        <v>0.31736111111111104</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="n">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
         <v>45965</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="8" t="n">
-        <v>0.378472222222222</v>
-      </c>
-      <c r="D13" s="8" t="n">
-        <v>0.461805555555556</v>
-      </c>
-      <c r="E13" s="9" t="n">
-        <f aca="false">D13-C13</f>
-        <v>0.0833333333333333</v>
+      <c r="C13" s="8">
+        <v>0.37847222222222199</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.46180555555555602</v>
+      </c>
+      <c r="E13" s="9">
+        <f t="shared" si="0"/>
+        <v>8.3333333333334036E-2</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="n">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>45965</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="8" t="n">
-        <v>0.572916666666667</v>
-      </c>
-      <c r="D14" s="8" t="n">
-        <v>0.607638888888889</v>
-      </c>
-      <c r="E14" s="9" t="n">
-        <f aca="false">D14-C14</f>
-        <v>0.0347222222222222</v>
+      <c r="C14" s="8">
+        <v>0.57291666666666696</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="E14" s="9">
+        <f t="shared" si="0"/>
+        <v>3.4722222222221988E-2</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="n">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
         <v>45967</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="15" t="n">
-        <v>0.420138888888889</v>
-      </c>
-      <c r="D15" s="15" t="n">
-        <v>0.58125</v>
-      </c>
-      <c r="E15" s="9" t="n">
-        <f aca="false">D15-C15</f>
-        <v>0.161111111111111</v>
+      <c r="C15" s="15">
+        <v>0.42013888888888901</v>
+      </c>
+      <c r="D15" s="15">
+        <v>0.58125000000000004</v>
+      </c>
+      <c r="E15" s="9">
+        <f t="shared" si="0"/>
+        <v>0.16111111111111104</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="n">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
         <v>45971</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="17" t="n">
+      <c r="C16" s="8">
         <v>0.5625</v>
       </c>
-      <c r="D16" s="17" t="n">
-        <v>0.660416666666667</v>
-      </c>
-      <c r="E16" s="9" t="n">
-        <f aca="false">D16-C16</f>
-        <v>0.0979166666666667</v>
+      <c r="D16" s="8">
+        <v>0.66041666666666698</v>
+      </c>
+      <c r="E16" s="9">
+        <f t="shared" si="0"/>
+        <v>9.7916666666666985E-2</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="9" t="n">
-        <f aca="false">D17-C17</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>45972</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.4375</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E17" s="9">
+        <f t="shared" si="0"/>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="9" t="n">
-        <f aca="false">D18-C18</f>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="9" t="n">
-        <f aca="false">D19-C19</f>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F19" s="10"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="9" t="n">
-        <f aca="false">D20-C20</f>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
       <c r="B21" s="7"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="9" t="n">
-        <f aca="false">D21-C21</f>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
       <c r="B22" s="7"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="9" t="n">
-        <f aca="false">D22-C22</f>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="9" t="n">
-        <f aca="false">D23-C23</f>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F23" s="10"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
       <c r="B24" s="7"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="9" t="n">
-        <f aca="false">D24-C24</f>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
       <c r="B25" s="7"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="9" t="n">
-        <f aca="false">D25-C25</f>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="16"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
       <c r="B26" s="7"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="9" t="n">
-        <f aca="false">D26-C26</f>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="16"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
       <c r="B27" s="7"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="9" t="n">
-        <f aca="false">D27-C27</f>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="16"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
       <c r="B28" s="7"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="9" t="n">
-        <f aca="false">D28-C28</f>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F28" s="10"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
       <c r="B29" s="7"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="9" t="n">
-        <f aca="false">D29-C29</f>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
       <c r="B30" s="7"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="9" t="n">
-        <f aca="false">D30-C30</f>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="16"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
       <c r="B31" s="7"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="9" t="n">
-        <f aca="false">D31-C31</f>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F31" s="10"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="16"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
       <c r="B32" s="7"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="9" t="n">
-        <f aca="false">D32-C32</f>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F32" s="10"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="16"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="9" t="n">
-        <f aca="false">D33-C33</f>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F33" s="10"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="16"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
       <c r="B34" s="7"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="9" t="n">
-        <f aca="false">D34-C34</f>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F34" s="10"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="16"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
       <c r="B35" s="7"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="9" t="n">
-        <f aca="false">D35-C35</f>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F35" s="10"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="9" t="n">
-        <f aca="false">D36-C36</f>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="9">
+        <f t="shared" ref="E36:E67" si="1">D36-C36</f>
         <v>0</v>
       </c>
       <c r="F36" s="10"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="9" t="n">
-        <f aca="false">D37-C37</f>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F37" s="10"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="9" t="n">
-        <f aca="false">D38-C38</f>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F38" s="10"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="9" t="n">
-        <f aca="false">D39-C39</f>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F39" s="10"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="9" t="n">
-        <f aca="false">D40-C40</f>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="9" t="n">
-        <f aca="false">D41-C41</f>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="9" t="n">
-        <f aca="false">D42-C42</f>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F42" s="10"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="9" t="n">
-        <f aca="false">D43-C43</f>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F43" s="10"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="9" t="n">
-        <f aca="false">D44-C44</f>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F44" s="10"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
-      <c r="E45" s="9" t="n">
-        <f aca="false">D45-C45</f>
+      <c r="E45" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F45" s="10"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
-      <c r="E46" s="9" t="n">
-        <f aca="false">D46-C46</f>
+      <c r="E46" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F46" s="10"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
-      <c r="E47" s="9" t="n">
-        <f aca="false">D47-C47</f>
+      <c r="E47" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F47" s="10"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
-      <c r="E48" s="9" t="n">
-        <f aca="false">D48-C48</f>
+      <c r="E48" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F48" s="10"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
-      <c r="E49" s="9" t="n">
-        <f aca="false">D49-C49</f>
+      <c r="E49" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F49" s="10"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
-      <c r="E50" s="9" t="n">
-        <f aca="false">D50-C50</f>
+      <c r="E50" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F50" s="10"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
-      <c r="E51" s="9" t="n">
-        <f aca="false">D51-C51</f>
+      <c r="E51" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F51" s="10"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
-      <c r="E52" s="9" t="n">
-        <f aca="false">D52-C52</f>
+      <c r="E52" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F52" s="10"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
-      <c r="E53" s="9" t="n">
-        <f aca="false">D53-C53</f>
+      <c r="E53" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F53" s="10"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
-      <c r="E54" s="9" t="n">
-        <f aca="false">D54-C54</f>
+      <c r="E54" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F54" s="10"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
-      <c r="E55" s="9" t="n">
-        <f aca="false">D55-C55</f>
+      <c r="E55" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F55" s="10"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
-      <c r="E56" s="9" t="n">
-        <f aca="false">D56-C56</f>
+      <c r="E56" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F56" s="10"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
-      <c r="E57" s="9" t="n">
-        <f aca="false">D57-C57</f>
+      <c r="E57" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F57" s="10"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
-      <c r="E58" s="9" t="n">
-        <f aca="false">D58-C58</f>
+      <c r="E58" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F58" s="10"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
-      <c r="E59" s="9" t="n">
-        <f aca="false">D59-C59</f>
+      <c r="E59" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F59" s="10"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
-      <c r="E60" s="9" t="n">
-        <f aca="false">D60-C60</f>
+      <c r="E60" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F60" s="10"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
-      <c r="E61" s="9" t="n">
-        <f aca="false">D61-C61</f>
+      <c r="E61" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F61" s="10"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
-      <c r="E62" s="9" t="n">
-        <f aca="false">D62-C62</f>
+      <c r="E62" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F62" s="10"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
-      <c r="E63" s="9" t="n">
-        <f aca="false">D63-C63</f>
+      <c r="E63" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F63" s="10"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
-      <c r="E64" s="9" t="n">
-        <f aca="false">D64-C64</f>
+      <c r="E64" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F64" s="10"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
-      <c r="E65" s="9" t="n">
-        <f aca="false">D65-C65</f>
+      <c r="E65" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F65" s="10"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
-      <c r="E66" s="9" t="n">
-        <f aca="false">D66-C66</f>
+      <c r="E66" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F66" s="10"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
-      <c r="E67" s="9" t="n">
-        <f aca="false">D67-C67</f>
+      <c r="E67" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F67" s="10"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
-      <c r="E68" s="9" t="n">
-        <f aca="false">D68-C68</f>
+      <c r="E68" s="9">
+        <f t="shared" ref="E68:E99" si="2">D68-C68</f>
         <v>0</v>
       </c>
       <c r="F68" s="10"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
-      <c r="E69" s="9" t="n">
-        <f aca="false">D69-C69</f>
+      <c r="E69" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F69" s="10"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
-      <c r="E70" s="9" t="n">
-        <f aca="false">D70-C70</f>
+      <c r="E70" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F70" s="10"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
-      <c r="E71" s="9" t="n">
-        <f aca="false">D71-C71</f>
+      <c r="E71" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F71" s="10"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
-      <c r="E72" s="9" t="n">
-        <f aca="false">D72-C72</f>
+      <c r="E72" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F72" s="10"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
-      <c r="E73" s="9" t="n">
-        <f aca="false">D73-C73</f>
+      <c r="E73" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F73" s="10"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
-      <c r="E74" s="9" t="n">
-        <f aca="false">D74-C74</f>
+      <c r="E74" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F74" s="10"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
-      <c r="E75" s="9" t="n">
-        <f aca="false">D75-C75</f>
+      <c r="E75" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F75" s="10"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
-      <c r="E76" s="9" t="n">
-        <f aca="false">D76-C76</f>
+      <c r="E76" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F76" s="10"/>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
-      <c r="E77" s="9" t="n">
-        <f aca="false">D77-C77</f>
+      <c r="E77" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F77" s="10"/>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
-      <c r="E78" s="9" t="n">
-        <f aca="false">D78-C78</f>
+      <c r="E78" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F78" s="10"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
-      <c r="E79" s="9" t="n">
-        <f aca="false">D79-C79</f>
+      <c r="E79" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F79" s="10"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
-      <c r="E80" s="9" t="n">
-        <f aca="false">D80-C80</f>
+      <c r="E80" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F80" s="10"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
-      <c r="E81" s="9" t="n">
-        <f aca="false">D81-C81</f>
+      <c r="E81" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F81" s="10"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
-      <c r="E82" s="9" t="n">
-        <f aca="false">D82-C82</f>
+      <c r="E82" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F82" s="10"/>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
-      <c r="E83" s="9" t="n">
-        <f aca="false">D83-C83</f>
+      <c r="E83" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F83" s="10"/>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
-      <c r="E84" s="9" t="n">
-        <f aca="false">D84-C84</f>
+      <c r="E84" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F84" s="10"/>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
-      <c r="E85" s="9" t="n">
-        <f aca="false">D85-C85</f>
+      <c r="E85" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F85" s="10"/>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
-      <c r="E86" s="9" t="n">
-        <f aca="false">D86-C86</f>
+      <c r="E86" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F86" s="10"/>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
-      <c r="E87" s="9" t="n">
-        <f aca="false">D87-C87</f>
+      <c r="E87" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F87" s="10"/>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
-      <c r="E88" s="9" t="n">
-        <f aca="false">D88-C88</f>
+      <c r="E88" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F88" s="10"/>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
-      <c r="E89" s="9" t="n">
-        <f aca="false">D89-C89</f>
+      <c r="E89" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F89" s="10"/>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
-      <c r="E90" s="9" t="n">
-        <f aca="false">D90-C90</f>
+      <c r="E90" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F90" s="10"/>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
-      <c r="E91" s="9" t="n">
-        <f aca="false">D91-C91</f>
+      <c r="E91" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F91" s="10"/>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
-      <c r="E92" s="9" t="n">
-        <f aca="false">D92-C92</f>
+      <c r="E92" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F92" s="10"/>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
-      <c r="E93" s="9" t="n">
-        <f aca="false">D93-C93</f>
+      <c r="E93" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F93" s="10"/>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
-      <c r="E94" s="9" t="n">
-        <f aca="false">D94-C94</f>
+      <c r="E94" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F94" s="10"/>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
-      <c r="E95" s="9" t="n">
-        <f aca="false">D95-C95</f>
+      <c r="E95" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F95" s="10"/>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
-      <c r="E96" s="9" t="n">
-        <f aca="false">D96-C96</f>
+      <c r="E96" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F96" s="10"/>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
-      <c r="E97" s="9" t="n">
-        <f aca="false">D97-C97</f>
+      <c r="E97" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F97" s="10"/>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
-      <c r="E98" s="9" t="n">
-        <f aca="false">D98-C98</f>
+      <c r="E98" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F98" s="10"/>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
-      <c r="E99" s="9" t="n">
-        <f aca="false">D99-C99</f>
+      <c r="E99" s="9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F99" s="10"/>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
-      <c r="E100" s="9" t="n">
-        <f aca="false">D100-C100</f>
+      <c r="E100" s="9">
+        <f t="shared" ref="E100:E131" si="3">D100-C100</f>
         <v>0</v>
       </c>
       <c r="F100" s="10"/>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
-      <c r="E101" s="9" t="n">
-        <f aca="false">D101-C101</f>
+      <c r="E101" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F101" s="10"/>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
-      <c r="E102" s="9" t="n">
-        <f aca="false">D102-C102</f>
+      <c r="E102" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F102" s="10"/>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
-      <c r="E103" s="9" t="n">
-        <f aca="false">D103-C103</f>
+      <c r="E103" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F103" s="10"/>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
-      <c r="E104" s="9" t="n">
-        <f aca="false">D104-C104</f>
+      <c r="E104" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F104" s="10"/>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
-      <c r="E105" s="9" t="n">
-        <f aca="false">D105-C105</f>
+      <c r="E105" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F105" s="10"/>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
-      <c r="E106" s="9" t="n">
-        <f aca="false">D106-C106</f>
+      <c r="E106" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F106" s="10"/>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
-      <c r="E107" s="9" t="n">
-        <f aca="false">D107-C107</f>
+      <c r="E107" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F107" s="10"/>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
-      <c r="E108" s="9" t="n">
-        <f aca="false">D108-C108</f>
+      <c r="E108" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F108" s="10"/>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
-      <c r="E109" s="9" t="n">
-        <f aca="false">D109-C109</f>
+      <c r="E109" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F109" s="10"/>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
-      <c r="E110" s="9" t="n">
-        <f aca="false">D110-C110</f>
+      <c r="E110" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F110" s="10"/>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
-      <c r="E111" s="9" t="n">
-        <f aca="false">D111-C111</f>
+      <c r="E111" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F111" s="10"/>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
-      <c r="E112" s="9" t="n">
-        <f aca="false">D112-C112</f>
+      <c r="E112" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F112" s="10"/>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
-      <c r="E113" s="9" t="n">
-        <f aca="false">D113-C113</f>
+      <c r="E113" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F113" s="10"/>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
-      <c r="E114" s="9" t="n">
-        <f aca="false">D114-C114</f>
+      <c r="E114" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F114" s="10"/>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
-      <c r="E115" s="9" t="n">
-        <f aca="false">D115-C115</f>
+      <c r="E115" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F115" s="10"/>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
-      <c r="E116" s="9" t="n">
-        <f aca="false">D116-C116</f>
+      <c r="E116" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F116" s="10"/>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
-      <c r="E117" s="9" t="n">
-        <f aca="false">D117-C117</f>
+      <c r="E117" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F117" s="10"/>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
-      <c r="E118" s="9" t="n">
-        <f aca="false">D118-C118</f>
+      <c r="E118" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F118" s="10"/>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
-      <c r="E119" s="9" t="n">
-        <f aca="false">D119-C119</f>
+      <c r="E119" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F119" s="10"/>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
-      <c r="E120" s="9" t="n">
-        <f aca="false">D120-C120</f>
+      <c r="E120" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F120" s="10"/>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
-      <c r="E121" s="9" t="n">
-        <f aca="false">D121-C121</f>
+      <c r="E121" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F121" s="10"/>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
-      <c r="E122" s="9" t="n">
-        <f aca="false">D122-C122</f>
+      <c r="E122" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F122" s="10"/>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
-      <c r="E123" s="9" t="n">
-        <f aca="false">D123-C123</f>
+      <c r="E123" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F123" s="10"/>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
-      <c r="E124" s="9" t="n">
-        <f aca="false">D124-C124</f>
+      <c r="E124" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F124" s="10"/>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
-      <c r="E125" s="9" t="n">
-        <f aca="false">D125-C125</f>
+      <c r="E125" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F125" s="10"/>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
-      <c r="E126" s="9" t="n">
-        <f aca="false">D126-C126</f>
+      <c r="E126" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F126" s="10"/>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="7"/>
       <c r="B127" s="7"/>
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
-      <c r="E127" s="9" t="n">
-        <f aca="false">D127-C127</f>
+      <c r="E127" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F127" s="10"/>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="7"/>
       <c r="B128" s="7"/>
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
-      <c r="E128" s="9" t="n">
-        <f aca="false">D128-C128</f>
+      <c r="E128" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F128" s="10"/>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="7"/>
       <c r="D129" s="7"/>
-      <c r="E129" s="9" t="n">
-        <f aca="false">D129-C129</f>
+      <c r="E129" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F129" s="10"/>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
       <c r="D130" s="7"/>
-      <c r="E130" s="9" t="n">
-        <f aca="false">D130-C130</f>
+      <c r="E130" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F130" s="10"/>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="7"/>
       <c r="D131" s="7"/>
-      <c r="E131" s="9" t="n">
-        <f aca="false">D131-C131</f>
+      <c r="E131" s="9">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F131" s="10"/>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
-      <c r="E132" s="9" t="n">
-        <f aca="false">D132-C132</f>
+      <c r="E132" s="9">
+        <f t="shared" ref="E132:E163" si="4">D132-C132</f>
         <v>0</v>
       </c>
       <c r="F132" s="10"/>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="7"/>
       <c r="D133" s="7"/>
-      <c r="E133" s="9" t="n">
-        <f aca="false">D133-C133</f>
+      <c r="E133" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F133" s="10"/>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
       <c r="D134" s="7"/>
-      <c r="E134" s="9" t="n">
-        <f aca="false">D134-C134</f>
+      <c r="E134" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F134" s="10"/>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
       <c r="D135" s="7"/>
-      <c r="E135" s="9" t="n">
-        <f aca="false">D135-C135</f>
+      <c r="E135" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F135" s="10"/>
     </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
       <c r="D136" s="7"/>
-      <c r="E136" s="9" t="n">
-        <f aca="false">D136-C136</f>
+      <c r="E136" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F136" s="10"/>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
       <c r="C137" s="7"/>
       <c r="D137" s="7"/>
-      <c r="E137" s="9" t="n">
-        <f aca="false">D137-C137</f>
+      <c r="E137" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F137" s="10"/>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
-      <c r="E138" s="9" t="n">
-        <f aca="false">D138-C138</f>
+      <c r="E138" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F138" s="10"/>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
       <c r="D139" s="7"/>
-      <c r="E139" s="9" t="n">
-        <f aca="false">D139-C139</f>
+      <c r="E139" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F139" s="10"/>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
-      <c r="E140" s="9" t="n">
-        <f aca="false">D140-C140</f>
+      <c r="E140" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F140" s="10"/>
     </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
       <c r="D141" s="7"/>
-      <c r="E141" s="9" t="n">
-        <f aca="false">D141-C141</f>
+      <c r="E141" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F141" s="10"/>
     </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="7"/>
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
-      <c r="E142" s="9" t="n">
-        <f aca="false">D142-C142</f>
+      <c r="E142" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F142" s="10"/>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="7"/>
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
       <c r="D143" s="7"/>
-      <c r="E143" s="9" t="n">
-        <f aca="false">D143-C143</f>
+      <c r="E143" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F143" s="10"/>
     </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="7"/>
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
-      <c r="E144" s="9" t="n">
-        <f aca="false">D144-C144</f>
+      <c r="E144" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F144" s="10"/>
     </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
       <c r="D145" s="7"/>
-      <c r="E145" s="9" t="n">
-        <f aca="false">D145-C145</f>
+      <c r="E145" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F145" s="10"/>
     </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="7"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
-      <c r="E146" s="9" t="n">
-        <f aca="false">D146-C146</f>
+      <c r="E146" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F146" s="10"/>
     </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="7"/>
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
-      <c r="E147" s="9" t="n">
-        <f aca="false">D147-C147</f>
+      <c r="E147" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F147" s="10"/>
     </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="7"/>
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
-      <c r="E148" s="9" t="n">
-        <f aca="false">D148-C148</f>
+      <c r="E148" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F148" s="10"/>
     </row>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="7"/>
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
       <c r="D149" s="7"/>
-      <c r="E149" s="9" t="n">
-        <f aca="false">D149-C149</f>
+      <c r="E149" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F149" s="10"/>
     </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="7"/>
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
       <c r="D150" s="7"/>
-      <c r="E150" s="9" t="n">
-        <f aca="false">D150-C150</f>
+      <c r="E150" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F150" s="10"/>
     </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="7"/>
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
       <c r="D151" s="7"/>
-      <c r="E151" s="9" t="n">
-        <f aca="false">D151-C151</f>
+      <c r="E151" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F151" s="10"/>
     </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="7"/>
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
-      <c r="E152" s="9" t="n">
-        <f aca="false">D152-C152</f>
+      <c r="E152" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F152" s="10"/>
     </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="7"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
-      <c r="E153" s="9" t="n">
-        <f aca="false">D153-C153</f>
+      <c r="E153" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F153" s="10"/>
     </row>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="7"/>
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
-      <c r="E154" s="9" t="n">
-        <f aca="false">D154-C154</f>
+      <c r="E154" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F154" s="10"/>
     </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="7"/>
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
       <c r="D155" s="7"/>
-      <c r="E155" s="9" t="n">
-        <f aca="false">D155-C155</f>
+      <c r="E155" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F155" s="10"/>
     </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="7"/>
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
       <c r="D156" s="7"/>
-      <c r="E156" s="9" t="n">
-        <f aca="false">D156-C156</f>
+      <c r="E156" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F156" s="10"/>
     </row>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="7"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
       <c r="D157" s="7"/>
-      <c r="E157" s="9" t="n">
-        <f aca="false">D157-C157</f>
+      <c r="E157" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F157" s="10"/>
     </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="7"/>
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
-      <c r="E158" s="9" t="n">
-        <f aca="false">D158-C158</f>
+      <c r="E158" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F158" s="10"/>
     </row>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="7"/>
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
-      <c r="E159" s="9" t="n">
-        <f aca="false">D159-C159</f>
+      <c r="E159" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F159" s="10"/>
     </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="7"/>
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
       <c r="D160" s="7"/>
-      <c r="E160" s="9" t="n">
-        <f aca="false">D160-C160</f>
+      <c r="E160" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F160" s="10"/>
     </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="7"/>
       <c r="B161" s="7"/>
       <c r="C161" s="7"/>
       <c r="D161" s="7"/>
-      <c r="E161" s="9" t="n">
-        <f aca="false">D161-C161</f>
+      <c r="E161" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F161" s="10"/>
     </row>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
       <c r="D162" s="7"/>
-      <c r="E162" s="9" t="n">
-        <f aca="false">D162-C162</f>
+      <c r="E162" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F162" s="10"/>
     </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="7"/>
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
       <c r="D163" s="7"/>
-      <c r="E163" s="9" t="n">
-        <f aca="false">D163-C163</f>
+      <c r="E163" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F163" s="10"/>
     </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
-      <c r="E164" s="9" t="n">
-        <f aca="false">D164-C164</f>
+      <c r="E164" s="9">
+        <f t="shared" ref="E164:E195" si="5">D164-C164</f>
         <v>0</v>
       </c>
       <c r="F164" s="10"/>
     </row>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="7"/>
       <c r="B165" s="7"/>
       <c r="C165" s="7"/>
       <c r="D165" s="7"/>
-      <c r="E165" s="9" t="n">
-        <f aca="false">D165-C165</f>
+      <c r="E165" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F165" s="10"/>
     </row>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
       <c r="D166" s="7"/>
-      <c r="E166" s="9" t="n">
-        <f aca="false">D166-C166</f>
+      <c r="E166" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F166" s="10"/>
     </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="7"/>
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
       <c r="D167" s="7"/>
-      <c r="E167" s="9" t="n">
-        <f aca="false">D167-C167</f>
+      <c r="E167" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F167" s="10"/>
     </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
       <c r="D168" s="7"/>
-      <c r="E168" s="9" t="n">
-        <f aca="false">D168-C168</f>
+      <c r="E168" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F168" s="10"/>
     </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="7"/>
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
       <c r="D169" s="7"/>
-      <c r="E169" s="9" t="n">
-        <f aca="false">D169-C169</f>
+      <c r="E169" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F169" s="10"/>
     </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
       <c r="D170" s="7"/>
-      <c r="E170" s="9" t="n">
-        <f aca="false">D170-C170</f>
+      <c r="E170" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F170" s="10"/>
     </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="7"/>
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
       <c r="D171" s="7"/>
-      <c r="E171" s="9" t="n">
-        <f aca="false">D171-C171</f>
+      <c r="E171" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F171" s="10"/>
     </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
       <c r="D172" s="7"/>
-      <c r="E172" s="9" t="n">
-        <f aca="false">D172-C172</f>
+      <c r="E172" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F172" s="10"/>
     </row>
-    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="7"/>
       <c r="B173" s="7"/>
       <c r="C173" s="7"/>
       <c r="D173" s="7"/>
-      <c r="E173" s="9" t="n">
-        <f aca="false">D173-C173</f>
+      <c r="E173" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F173" s="10"/>
     </row>
-    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="7"/>
       <c r="B174" s="7"/>
       <c r="C174" s="7"/>
       <c r="D174" s="7"/>
-      <c r="E174" s="9" t="n">
-        <f aca="false">D174-C174</f>
+      <c r="E174" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F174" s="10"/>
     </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="7"/>
       <c r="B175" s="7"/>
       <c r="C175" s="7"/>
       <c r="D175" s="7"/>
-      <c r="E175" s="9" t="n">
-        <f aca="false">D175-C175</f>
+      <c r="E175" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F175" s="10"/>
     </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="7"/>
       <c r="B176" s="7"/>
       <c r="C176" s="7"/>
       <c r="D176" s="7"/>
-      <c r="E176" s="9" t="n">
-        <f aca="false">D176-C176</f>
+      <c r="E176" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F176" s="10"/>
     </row>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="7"/>
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
       <c r="D177" s="7"/>
-      <c r="E177" s="9" t="n">
-        <f aca="false">D177-C177</f>
+      <c r="E177" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F177" s="10"/>
     </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="7"/>
       <c r="B178" s="7"/>
       <c r="C178" s="7"/>
       <c r="D178" s="7"/>
-      <c r="E178" s="9" t="n">
-        <f aca="false">D178-C178</f>
+      <c r="E178" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F178" s="10"/>
     </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="7"/>
       <c r="B179" s="7"/>
       <c r="C179" s="7"/>
       <c r="D179" s="7"/>
-      <c r="E179" s="9" t="n">
-        <f aca="false">D179-C179</f>
+      <c r="E179" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F179" s="10"/>
     </row>
-    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="7"/>
       <c r="B180" s="7"/>
       <c r="C180" s="7"/>
       <c r="D180" s="7"/>
-      <c r="E180" s="9" t="n">
-        <f aca="false">D180-C180</f>
+      <c r="E180" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F180" s="10"/>
     </row>
-    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="7"/>
       <c r="B181" s="7"/>
       <c r="C181" s="7"/>
       <c r="D181" s="7"/>
-      <c r="E181" s="9" t="n">
-        <f aca="false">D181-C181</f>
+      <c r="E181" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F181" s="10"/>
     </row>
-    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="7"/>
       <c r="B182" s="7"/>
       <c r="C182" s="7"/>
       <c r="D182" s="7"/>
-      <c r="E182" s="9" t="n">
-        <f aca="false">D182-C182</f>
+      <c r="E182" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F182" s="10"/>
     </row>
-    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="7"/>
       <c r="B183" s="7"/>
       <c r="C183" s="7"/>
       <c r="D183" s="7"/>
-      <c r="E183" s="9" t="n">
-        <f aca="false">D183-C183</f>
+      <c r="E183" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F183" s="10"/>
     </row>
-    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="7"/>
       <c r="B184" s="7"/>
       <c r="C184" s="7"/>
       <c r="D184" s="7"/>
-      <c r="E184" s="9" t="n">
-        <f aca="false">D184-C184</f>
+      <c r="E184" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F184" s="10"/>
     </row>
-    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="7"/>
       <c r="B185" s="7"/>
       <c r="C185" s="7"/>
       <c r="D185" s="7"/>
-      <c r="E185" s="9" t="n">
-        <f aca="false">D185-C185</f>
+      <c r="E185" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F185" s="10"/>
     </row>
-    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="7"/>
       <c r="B186" s="7"/>
       <c r="C186" s="7"/>
       <c r="D186" s="7"/>
-      <c r="E186" s="9" t="n">
-        <f aca="false">D186-C186</f>
+      <c r="E186" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F186" s="10"/>
     </row>
-    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="7"/>
       <c r="B187" s="7"/>
       <c r="C187" s="7"/>
       <c r="D187" s="7"/>
-      <c r="E187" s="9" t="n">
-        <f aca="false">D187-C187</f>
+      <c r="E187" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F187" s="10"/>
     </row>
-    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="7"/>
       <c r="B188" s="7"/>
       <c r="C188" s="7"/>
       <c r="D188" s="7"/>
-      <c r="E188" s="9" t="n">
-        <f aca="false">D188-C188</f>
+      <c r="E188" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F188" s="10"/>
     </row>
-    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="7"/>
       <c r="B189" s="7"/>
       <c r="C189" s="7"/>
       <c r="D189" s="7"/>
-      <c r="E189" s="9" t="n">
-        <f aca="false">D189-C189</f>
+      <c r="E189" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F189" s="10"/>
     </row>
-    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="7"/>
       <c r="B190" s="7"/>
       <c r="C190" s="7"/>
       <c r="D190" s="7"/>
-      <c r="E190" s="9" t="n">
-        <f aca="false">D190-C190</f>
+      <c r="E190" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F190" s="10"/>
     </row>
-    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="7"/>
       <c r="B191" s="7"/>
       <c r="C191" s="7"/>
       <c r="D191" s="7"/>
-      <c r="E191" s="9" t="n">
-        <f aca="false">D191-C191</f>
+      <c r="E191" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F191" s="10"/>
     </row>
-    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="7"/>
       <c r="B192" s="7"/>
       <c r="C192" s="7"/>
       <c r="D192" s="7"/>
-      <c r="E192" s="9" t="n">
-        <f aca="false">D192-C192</f>
+      <c r="E192" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F192" s="10"/>
     </row>
-    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="7"/>
       <c r="B193" s="7"/>
       <c r="C193" s="7"/>
       <c r="D193" s="7"/>
-      <c r="E193" s="9" t="n">
-        <f aca="false">D193-C193</f>
+      <c r="E193" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F193" s="10"/>
     </row>
-    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="7"/>
       <c r="B194" s="7"/>
       <c r="C194" s="7"/>
       <c r="D194" s="7"/>
-      <c r="E194" s="9" t="n">
-        <f aca="false">D194-C194</f>
+      <c r="E194" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F194" s="10"/>
     </row>
-    <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="7"/>
       <c r="B195" s="7"/>
       <c r="C195" s="7"/>
       <c r="D195" s="7"/>
-      <c r="E195" s="9" t="n">
-        <f aca="false">D195-C195</f>
+      <c r="E195" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F195" s="10"/>
     </row>
-    <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="7"/>
       <c r="B196" s="7"/>
       <c r="C196" s="7"/>
       <c r="D196" s="7"/>
-      <c r="E196" s="9" t="n">
-        <f aca="false">D196-C196</f>
+      <c r="E196" s="9">
+        <f t="shared" ref="E196:E227" si="6">D196-C196</f>
         <v>0</v>
       </c>
       <c r="F196" s="10"/>
     </row>
-    <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="7"/>
       <c r="B197" s="7"/>
       <c r="C197" s="7"/>
       <c r="D197" s="7"/>
-      <c r="E197" s="9" t="n">
-        <f aca="false">D197-C197</f>
+      <c r="E197" s="9">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F197" s="10"/>
     </row>
-    <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="7"/>
       <c r="B198" s="7"/>
       <c r="C198" s="7"/>
       <c r="D198" s="7"/>
-      <c r="E198" s="9" t="n">
-        <f aca="false">D198-C198</f>
+      <c r="E198" s="9">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F198" s="10"/>
     </row>
-    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="7"/>
       <c r="B199" s="7"/>
       <c r="C199" s="7"/>
       <c r="D199" s="7"/>
-      <c r="E199" s="9" t="n">
-        <f aca="false">D199-C199</f>
+      <c r="E199" s="9">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F199" s="10"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>